<commit_message>
Easy Rust index updated
</commit_message>
<xml_diff>
--- a/toc_easyrust_playlist/TOC - Easy Rust in Korean.xlsx
+++ b/toc_easyrust_playlist/TOC - Easy Rust in Korean.xlsx
@@ -480,7 +480,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D178"/>
+  <dimension ref="A1:D181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,9 +529,9 @@
       </c>
       <c r="C2" s="10" t="inlineStr">
         <is>
-          <t>1 day, 3:50:56
-100256 secs
-175 videos</t>
+          <t>1 day, 4:23:59
+102239 secs
+179 videos</t>
         </is>
       </c>
       <c r="D2" s="10" t="inlineStr">
@@ -4407,6 +4407,72 @@
       <c r="D178" s="10" t="inlineStr">
         <is>
           <t>2022-05-21T06:41:56Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="12" t="inlineStr">
+        <is>
+          <t>173 User input</t>
+        </is>
+      </c>
+      <c r="B179" s="13" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=SsUVRbmHoZE</t>
+        </is>
+      </c>
+      <c r="C179" s="14" t="inlineStr">
+        <is>
+          <t>00:10:20</t>
+        </is>
+      </c>
+      <c r="D179" s="10" t="inlineStr">
+        <is>
+          <t>2022-06-19T07:09:38Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="12" t="inlineStr">
+        <is>
+          <t>174 Program arguments</t>
+        </is>
+      </c>
+      <c r="B180" s="13" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=PLqe4vD2iVg</t>
+        </is>
+      </c>
+      <c r="C180" s="14" t="inlineStr">
+        <is>
+          <t>00:13:12</t>
+        </is>
+      </c>
+      <c r="D180" s="10" t="inlineStr">
+        <is>
+          <t>2022-06-19T07:11:45Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="12" t="inlineStr">
+        <is>
+          <t>175 Statics in Rust 1.63</t>
+        </is>
+      </c>
+      <c r="B181" s="13" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=T5OwV2HaH9E</t>
+        </is>
+      </c>
+      <c r="C181" s="14" t="inlineStr">
+        <is>
+          <t>00:09:31</t>
+        </is>
+      </c>
+      <c r="D181" s="10" t="inlineStr">
+        <is>
+          <t>2022-06-26T06:40:20Z</t>
         </is>
       </c>
     </row>
@@ -4588,6 +4654,9 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B176" r:id="rId174"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B177" r:id="rId175"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B178" r:id="rId176"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B179" r:id="rId177"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B180" r:id="rId178"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B181" r:id="rId179"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
filter Only EasyRust contents
</commit_message>
<xml_diff>
--- a/toc_easyrust_playlist/TOC - Easy Rust in Korean.xlsx
+++ b/toc_easyrust_playlist/TOC - Easy Rust in Korean.xlsx
@@ -480,7 +480,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D184"/>
+  <dimension ref="A1:D180"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,8 +529,8 @@
       </c>
       <c r="C2" s="10" t="inlineStr">
         <is>
-          <t>1 day, 4:45:36
-103536 secs
+          <t>1 day, 3:16:59
+98219 secs
 181 videos</t>
         </is>
       </c>
@@ -565,3980 +565,3896 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="12" t="n"/>
+      <c r="A4" s="12" t="inlineStr">
+        <is>
+          <t>001 Intro</t>
+        </is>
+      </c>
       <c r="B4" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=1buxquPfWLk</t>
+          <t>https://www.youtube.com/watch?v=W9DO6m8JSSs</t>
         </is>
       </c>
       <c r="C4" s="14" t="inlineStr">
         <is>
-          <t>00:08:05</t>
+          <t>00:06:09</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>2022-05-21T05:38:14Z</t>
+          <t>2021-11-22T12:11:01Z</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="12" t="inlineStr">
         <is>
-          <t>/ Us/ Using Rust to make a keyboard for hieroglyphs!</t>
+          <t>002 Comments</t>
         </is>
       </c>
       <c r="B5" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=1CXNgl_4fas</t>
+          <t>https://www.youtube.com/watch?v=x7GlQjh2aSw</t>
         </is>
       </c>
       <c r="C5" s="14" t="inlineStr">
         <is>
-          <t>01:18:01</t>
+          <t>00:04:57</t>
         </is>
       </c>
       <c r="D5" s="10" t="inlineStr">
         <is>
-          <t>2022-05-07T04:00:58Z</t>
+          <t>2021-11-22T12:14:40Z</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="12" t="inlineStr">
         <is>
-          <t>001 Intro</t>
+          <t>003 Integers</t>
         </is>
       </c>
       <c r="B6" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=W9DO6m8JSSs</t>
+          <t>https://www.youtube.com/watch?v=dEMYR99YIao</t>
         </is>
       </c>
       <c r="C6" s="14" t="inlineStr">
         <is>
-          <t>00:06:09</t>
+          <t>00:08:13</t>
         </is>
       </c>
       <c r="D6" s="10" t="inlineStr">
         <is>
-          <t>2021-11-22T12:11:01Z</t>
+          <t>2021-11-22T12:15:56Z</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="12" t="inlineStr">
         <is>
-          <t>002 Comments</t>
+          <t>004 Chars</t>
         </is>
       </c>
       <c r="B7" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=x7GlQjh2aSw</t>
+          <t>https://www.youtube.com/watch?v=yR33X2Ik9W0</t>
         </is>
       </c>
       <c r="C7" s="14" t="inlineStr">
         <is>
-          <t>00:04:57</t>
+          <t>00:08:01</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>2021-11-22T12:14:40Z</t>
+          <t>2021-11-22T12:17:12Z</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="12" t="inlineStr">
         <is>
-          <t>003 Integers</t>
+          <t>005 Chars 2</t>
         </is>
       </c>
       <c r="B8" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=dEMYR99YIao</t>
+          <t>https://www.youtube.com/watch?v=fpDTY7UuPaw</t>
         </is>
       </c>
       <c r="C8" s="14" t="inlineStr">
         <is>
-          <t>00:08:13</t>
+          <t>00:07:37</t>
         </is>
       </c>
       <c r="D8" s="10" t="inlineStr">
         <is>
-          <t>2021-11-22T12:15:56Z</t>
+          <t>2021-11-22T12:18:01Z</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="12" t="inlineStr">
         <is>
-          <t>004 Chars</t>
+          <t>006 Floats</t>
         </is>
       </c>
       <c r="B9" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=yR33X2Ik9W0</t>
+          <t>https://www.youtube.com/watch?v=qHEFgX-zCSs</t>
         </is>
       </c>
       <c r="C9" s="14" t="inlineStr">
         <is>
-          <t>00:08:01</t>
+          <t>00:04:19</t>
         </is>
       </c>
       <c r="D9" s="10" t="inlineStr">
         <is>
-          <t>2021-11-22T12:17:12Z</t>
+          <t>2021-11-24T09:52:55Z</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="12" t="inlineStr">
         <is>
-          <t>005 Chars 2</t>
+          <t>007 println!</t>
         </is>
       </c>
       <c r="B10" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=fpDTY7UuPaw</t>
+          <t>https://www.youtube.com/watch?v=jpLwve-7Cjg</t>
         </is>
       </c>
       <c r="C10" s="14" t="inlineStr">
         <is>
-          <t>00:07:37</t>
+          <t>00:06:23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>2021-11-22T12:18:01Z</t>
+          <t>2021-11-25T08:23:15Z</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="12" t="inlineStr">
         <is>
-          <t>006 Floats</t>
+          <t>008 println! 2</t>
         </is>
       </c>
       <c r="B11" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=qHEFgX-zCSs</t>
+          <t>https://www.youtube.com/watch?v=f-UCvEs7J3I</t>
         </is>
       </c>
       <c r="C11" s="14" t="inlineStr">
         <is>
-          <t>00:04:19</t>
+          <t>00:06:26</t>
         </is>
       </c>
       <c r="D11" s="10" t="inlineStr">
         <is>
-          <t>2021-11-24T09:52:55Z</t>
+          <t>2021-11-26T08:59:48Z</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="12" t="inlineStr">
         <is>
-          <t>007 println!</t>
+          <t>009 semicolon, unit type</t>
         </is>
       </c>
       <c r="B12" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=jpLwve-7Cjg</t>
+          <t>https://www.youtube.com/watch?v=jxuNkx4XCXg</t>
         </is>
       </c>
       <c r="C12" s="14" t="inlineStr">
         <is>
-          <t>00:06:23</t>
+          <t>00:06:54</t>
         </is>
       </c>
       <c r="D12" s="10" t="inlineStr">
         <is>
-          <t>2021-11-25T08:23:15Z</t>
+          <t>2021-11-27T06:38:18Z</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="12" t="inlineStr">
         <is>
-          <t>008 println! 2</t>
+          <t>010 functions, code blocks</t>
         </is>
       </c>
       <c r="B13" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=f-UCvEs7J3I</t>
+          <t>https://www.youtube.com/watch?v=XfWW4XzT17M</t>
         </is>
       </c>
       <c r="C13" s="14" t="inlineStr">
         <is>
-          <t>00:06:26</t>
+          <t>00:05:48</t>
         </is>
       </c>
       <c r="D13" s="10" t="inlineStr">
         <is>
-          <t>2021-11-26T08:59:48Z</t>
+          <t>2021-11-27T06:43:09Z</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="12" t="inlineStr">
         <is>
-          <t>009 semicolon, unit type</t>
+          <t>011 mutability and shadowing</t>
         </is>
       </c>
       <c r="B14" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=jxuNkx4XCXg</t>
+          <t>https://www.youtube.com/watch?v=uHuMJw73ukg</t>
         </is>
       </c>
       <c r="C14" s="14" t="inlineStr">
         <is>
-          <t>00:06:54</t>
+          <t>00:08:59</t>
         </is>
       </c>
       <c r="D14" s="10" t="inlineStr">
         <is>
-          <t>2021-11-27T06:38:18Z</t>
+          <t>2021-11-27T06:45:17Z</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="12" t="inlineStr">
         <is>
-          <t>010 functions, code blocks</t>
+          <t>012 memory + references</t>
         </is>
       </c>
       <c r="B15" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=XfWW4XzT17M</t>
+          <t>https://www.youtube.com/watch?v=dRunrgbBNKQ</t>
         </is>
       </c>
       <c r="C15" s="14" t="inlineStr">
         <is>
-          <t>00:05:48</t>
+          <t>00:06:06</t>
         </is>
       </c>
       <c r="D15" s="10" t="inlineStr">
         <is>
-          <t>2021-11-27T06:43:09Z</t>
+          <t>2021-12-02T03:17:43Z</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="12" t="inlineStr">
         <is>
-          <t>011 mutability and shadowing</t>
+          <t>013 fancy printing</t>
         </is>
       </c>
       <c r="B16" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=uHuMJw73ukg</t>
+          <t>https://www.youtube.com/watch?v=RuTElptHqdg</t>
         </is>
       </c>
       <c r="C16" s="14" t="inlineStr">
         <is>
-          <t>00:08:59</t>
+          <t>00:11:26</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>2021-11-27T06:45:17Z</t>
+          <t>2021-11-27T06:53:04Z</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="12" t="inlineStr">
         <is>
-          <t>012 memory + references</t>
+          <t>014 String and &amp;str</t>
         </is>
       </c>
       <c r="B17" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=dRunrgbBNKQ</t>
+          <t>https://www.youtube.com/watch?v=es_LX2vdCbo</t>
         </is>
       </c>
       <c r="C17" s="14" t="inlineStr">
         <is>
-          <t>00:06:06</t>
+          <t>00:06:50</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>2021-12-02T03:17:43Z</t>
+          <t>2021-12-02T03:20:19Z</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="12" t="inlineStr">
         <is>
-          <t>013 fancy printing</t>
+          <t>015 String methods</t>
         </is>
       </c>
       <c r="B18" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=RuTElptHqdg</t>
+          <t>https://www.youtube.com/watch?v=MebpscwF7L4</t>
         </is>
       </c>
       <c r="C18" s="14" t="inlineStr">
         <is>
-          <t>00:11:26</t>
+          <t>00:09:35</t>
         </is>
       </c>
       <c r="D18" s="10" t="inlineStr">
         <is>
-          <t>2021-11-27T06:53:04Z</t>
+          <t>2021-12-02T04:56:05Z</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="12" t="inlineStr">
         <is>
-          <t>014 String and &amp;str</t>
+          <t>016 const and static</t>
         </is>
       </c>
       <c r="B19" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=es_LX2vdCbo</t>
+          <t>https://www.youtube.com/watch?v=E48iJShSi7s</t>
         </is>
       </c>
       <c r="C19" s="14" t="inlineStr">
         <is>
-          <t>00:06:50</t>
+          <t>00:09:06</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>2021-12-02T03:20:19Z</t>
+          <t>2021-12-04T06:43:07Z</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="12" t="inlineStr">
         <is>
-          <t>015 String methods</t>
+          <t>017 returning a reference</t>
         </is>
       </c>
       <c r="B20" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=MebpscwF7L4</t>
+          <t>https://www.youtube.com/watch?v=JUowp7swKP4</t>
         </is>
       </c>
       <c r="C20" s="14" t="inlineStr">
         <is>
-          <t>00:09:35</t>
+          <t>00:05:09</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>2021-12-02T04:56:05Z</t>
+          <t>2021-12-04T07:31:22Z</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="12" t="inlineStr">
         <is>
-          <t>016 const and static</t>
+          <t>018 mutable references</t>
         </is>
       </c>
       <c r="B21" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=E48iJShSi7s</t>
+          <t>https://www.youtube.com/watch?v=1ZOf5MD-L3E</t>
         </is>
       </c>
       <c r="C21" s="14" t="inlineStr">
         <is>
-          <t>00:09:06</t>
+          <t>00:07:36</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
-          <t>2021-12-04T06:43:07Z</t>
+          <t>2021-12-04T07:33:07Z</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="12" t="inlineStr">
         <is>
-          <t>017 returning a reference</t>
+          <t>019 references and shadowing</t>
         </is>
       </c>
       <c r="B22" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=JUowp7swKP4</t>
+          <t>https://www.youtube.com/watch?v=oOXM9Aafem8</t>
         </is>
       </c>
       <c r="C22" s="14" t="inlineStr">
         <is>
-          <t>00:05:09</t>
+          <t>00:05:55</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>2021-12-04T07:31:22Z</t>
+          <t>2021-12-04T07:39:04Z</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="12" t="inlineStr">
         <is>
-          <t>018 mutable references</t>
+          <t>020 references in functions</t>
         </is>
       </c>
       <c r="B23" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=1ZOf5MD-L3E</t>
+          <t>https://www.youtube.com/watch?v=vSJXJfJgokg</t>
         </is>
       </c>
       <c r="C23" s="14" t="inlineStr">
         <is>
-          <t>00:07:36</t>
+          <t>00:04:42</t>
         </is>
       </c>
       <c r="D23" s="10" t="inlineStr">
         <is>
-          <t>2021-12-04T07:33:07Z</t>
+          <t>2021-12-04T07:44:12Z</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="12" t="inlineStr">
         <is>
-          <t>019 references and shadowing</t>
+          <t>021 mutable references and mut in functions</t>
         </is>
       </c>
       <c r="B24" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=oOXM9Aafem8</t>
+          <t>https://www.youtube.com/watch?v=W67u80b84oM</t>
         </is>
       </c>
       <c r="C24" s="14" t="inlineStr">
         <is>
-          <t>00:05:55</t>
+          <t>00:06:17</t>
         </is>
       </c>
       <c r="D24" s="10" t="inlineStr">
         <is>
-          <t>2021-12-04T07:39:04Z</t>
+          <t>2021-12-04T07:46:39Z</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="12" t="inlineStr">
         <is>
-          <t>020 references in functions</t>
+          <t>022 copy and clone</t>
         </is>
       </c>
       <c r="B25" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=vSJXJfJgokg</t>
+          <t>https://www.youtube.com/watch?v=dzUnIvKMlMc</t>
         </is>
       </c>
       <c r="C25" s="14" t="inlineStr">
         <is>
-          <t>00:04:42</t>
+          <t>00:06:15</t>
         </is>
       </c>
       <c r="D25" s="10" t="inlineStr">
         <is>
-          <t>2021-12-04T07:44:12Z</t>
+          <t>2021-12-04T07:47:40Z</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="12" t="inlineStr">
         <is>
-          <t>021 mutable references and mut in functions</t>
+          <t>023 uninitialized variables and for loops</t>
         </is>
       </c>
       <c r="B26" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=W67u80b84oM</t>
+          <t>https://www.youtube.com/watch?v=7o5mLFRf_uc</t>
         </is>
       </c>
       <c r="C26" s="14" t="inlineStr">
         <is>
-          <t>00:06:17</t>
+          <t>00:08:32</t>
         </is>
       </c>
       <c r="D26" s="10" t="inlineStr">
         <is>
-          <t>2021-12-04T07:46:39Z</t>
+          <t>2021-12-11T09:23:17Z</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="12" t="inlineStr">
         <is>
-          <t>022 copy and clone</t>
+          <t>024 arrays</t>
         </is>
       </c>
       <c r="B27" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=dzUnIvKMlMc</t>
+          <t>https://www.youtube.com/watch?v=bvTIx2I8g2A</t>
         </is>
       </c>
       <c r="C27" s="14" t="inlineStr">
         <is>
-          <t>00:06:15</t>
+          <t>00:07:46</t>
         </is>
       </c>
       <c r="D27" s="10" t="inlineStr">
         <is>
-          <t>2021-12-04T07:47:40Z</t>
+          <t>2021-12-11T09:26:57Z</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="12" t="inlineStr">
         <is>
-          <t>023 uninitialized variables and for loops</t>
+          <t>025 slices</t>
         </is>
       </c>
       <c r="B28" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=7o5mLFRf_uc</t>
+          <t>https://www.youtube.com/watch?v=l-hAfuaAnaU</t>
         </is>
       </c>
       <c r="C28" s="14" t="inlineStr">
         <is>
-          <t>00:08:32</t>
+          <t>00:05:47</t>
         </is>
       </c>
       <c r="D28" s="10" t="inlineStr">
         <is>
-          <t>2021-12-11T09:23:17Z</t>
+          <t>2021-12-11T09:29:25Z</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="12" t="inlineStr">
         <is>
-          <t>024 arrays</t>
+          <t>026 Vecs</t>
         </is>
       </c>
       <c r="B29" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=bvTIx2I8g2A</t>
+          <t>https://www.youtube.com/watch?v=J5qMnp0F-Co</t>
         </is>
       </c>
       <c r="C29" s="14" t="inlineStr">
         <is>
-          <t>00:07:46</t>
+          <t>00:06:08</t>
         </is>
       </c>
       <c r="D29" s="10" t="inlineStr">
         <is>
-          <t>2021-12-11T09:26:57Z</t>
+          <t>2021-12-11T09:31:23Z</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="12" t="inlineStr">
         <is>
-          <t>025 slices</t>
+          <t>027 From and Into</t>
         </is>
       </c>
       <c r="B30" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=l-hAfuaAnaU</t>
+          <t>https://www.youtube.com/watch?v=ZFRFKson38c</t>
         </is>
       </c>
       <c r="C30" s="14" t="inlineStr">
         <is>
-          <t>00:05:47</t>
+          <t>00:06:47</t>
         </is>
       </c>
       <c r="D30" s="10" t="inlineStr">
         <is>
-          <t>2021-12-11T09:29:25Z</t>
+          <t>2021-12-11T09:33:13Z</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="12" t="inlineStr">
         <is>
-          <t>026 Vecs</t>
+          <t>028 Tuples and destructuring</t>
         </is>
       </c>
       <c r="B31" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=J5qMnp0F-Co</t>
+          <t>https://www.youtube.com/watch?v=3A7YiwUEzek</t>
         </is>
       </c>
       <c r="C31" s="14" t="inlineStr">
         <is>
-          <t>00:06:08</t>
+          <t>00:10:00</t>
         </is>
       </c>
       <c r="D31" s="10" t="inlineStr">
         <is>
-          <t>2021-12-11T09:31:23Z</t>
+          <t>2021-12-11T09:35:00Z</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="12" t="inlineStr">
         <is>
-          <t>027 From and Into</t>
+          <t>029 Control flow and match</t>
         </is>
       </c>
       <c r="B32" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=ZFRFKson38c</t>
+          <t>https://www.youtube.com/watch?v=nCvHim8rGik</t>
         </is>
       </c>
       <c r="C32" s="14" t="inlineStr">
         <is>
-          <t>00:06:47</t>
+          <t>00:07:22</t>
         </is>
       </c>
       <c r="D32" s="10" t="inlineStr">
         <is>
-          <t>2021-12-11T09:33:13Z</t>
+          <t>2021-12-11T09:36:25Z</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="12" t="inlineStr">
         <is>
-          <t>028 Tuples and destructuring</t>
+          <t>030 Match statements</t>
         </is>
       </c>
       <c r="B33" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=3A7YiwUEzek</t>
+          <t>https://www.youtube.com/watch?v=SEpPI1JMIuc</t>
         </is>
       </c>
       <c r="C33" s="14" t="inlineStr">
         <is>
-          <t>00:10:00</t>
+          <t>00:08:58</t>
         </is>
       </c>
       <c r="D33" s="10" t="inlineStr">
         <is>
-          <t>2021-12-11T09:35:00Z</t>
+          <t>2021-12-18T04:08:33Z</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="12" t="inlineStr">
         <is>
-          <t>029 Control flow and match</t>
+          <t>031 More match statements</t>
         </is>
       </c>
       <c r="B34" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=nCvHim8rGik</t>
+          <t>https://www.youtube.com/watch?v=wJCOdCDTuDc</t>
         </is>
       </c>
       <c r="C34" s="14" t="inlineStr">
         <is>
-          <t>00:07:22</t>
+          <t>00:10:21</t>
         </is>
       </c>
       <c r="D34" s="10" t="inlineStr">
         <is>
-          <t>2021-12-11T09:36:25Z</t>
+          <t>2021-12-18T13:18:20Z</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="12" t="inlineStr">
         <is>
-          <t>030 Match statements</t>
+          <t>032 Structs</t>
         </is>
       </c>
       <c r="B35" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=SEpPI1JMIuc</t>
+          <t>https://www.youtube.com/watch?v=UVeg7xzYXWc</t>
         </is>
       </c>
       <c r="C35" s="14" t="inlineStr">
         <is>
-          <t>00:08:58</t>
+          <t>00:11:08</t>
         </is>
       </c>
       <c r="D35" s="10" t="inlineStr">
         <is>
-          <t>2021-12-18T04:08:33Z</t>
+          <t>2021-12-18T13:20:31Z</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="12" t="inlineStr">
         <is>
-          <t>031 More match statements</t>
+          <t>033 Struct size</t>
         </is>
       </c>
       <c r="B36" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=wJCOdCDTuDc</t>
+          <t>https://www.youtube.com/watch?v=5128Pe6EI_M</t>
         </is>
       </c>
       <c r="C36" s="14" t="inlineStr">
         <is>
-          <t>00:10:21</t>
+          <t>00:10:26</t>
         </is>
       </c>
       <c r="D36" s="10" t="inlineStr">
         <is>
-          <t>2021-12-18T13:18:20Z</t>
+          <t>2021-12-20T13:50:19Z</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="12" t="inlineStr">
         <is>
-          <t>032 Structs</t>
+          <t>034 Enums</t>
         </is>
       </c>
       <c r="B37" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=UVeg7xzYXWc</t>
+          <t>https://www.youtube.com/watch?v=eapws_zsumA</t>
         </is>
       </c>
       <c r="C37" s="14" t="inlineStr">
         <is>
-          <t>00:11:08</t>
+          <t>00:07:37</t>
         </is>
       </c>
       <c r="D37" s="10" t="inlineStr">
         <is>
-          <t>2021-12-18T13:20:31Z</t>
+          <t>2021-12-20T14:09:18Z</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="12" t="inlineStr">
         <is>
-          <t>033 Struct size</t>
+          <t>035 Enums 2</t>
         </is>
       </c>
       <c r="B38" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=5128Pe6EI_M</t>
+          <t>https://www.youtube.com/watch?v=7J1RvzHEVPo</t>
         </is>
       </c>
       <c r="C38" s="14" t="inlineStr">
         <is>
-          <t>00:10:26</t>
+          <t>00:07:45</t>
         </is>
       </c>
       <c r="D38" s="10" t="inlineStr">
         <is>
-          <t>2021-12-20T13:50:19Z</t>
+          <t>2021-12-20T14:15:29Z</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="12" t="inlineStr">
         <is>
-          <t>034 Enums</t>
+          <t>036 Enums 3</t>
         </is>
       </c>
       <c r="B39" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=eapws_zsumA</t>
+          <t>https://www.youtube.com/watch?v=TNrEaNtsoZw</t>
         </is>
       </c>
       <c r="C39" s="14" t="inlineStr">
         <is>
-          <t>00:07:37</t>
+          <t>00:11:57</t>
         </is>
       </c>
       <c r="D39" s="10" t="inlineStr">
         <is>
-          <t>2021-12-20T14:09:18Z</t>
+          <t>2021-12-20T14:16:50Z</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="12" t="inlineStr">
         <is>
-          <t>035 Enums 2</t>
+          <t>037 Loops</t>
         </is>
       </c>
       <c r="B40" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=7J1RvzHEVPo</t>
+          <t>https://www.youtube.com/watch?v=11yZ9n7m0uU</t>
         </is>
       </c>
       <c r="C40" s="14" t="inlineStr">
         <is>
-          <t>00:07:45</t>
+          <t>00:06:42</t>
         </is>
       </c>
       <c r="D40" s="10" t="inlineStr">
         <is>
-          <t>2021-12-20T14:15:29Z</t>
+          <t>2021-12-25T04:29:15Z</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="12" t="inlineStr">
         <is>
-          <t>036 Enums 3</t>
+          <t>038 More loops</t>
         </is>
       </c>
       <c r="B41" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=TNrEaNtsoZw</t>
+          <t>https://www.youtube.com/watch?v=1xhe1eQRKsk</t>
         </is>
       </c>
       <c r="C41" s="14" t="inlineStr">
         <is>
-          <t>00:11:57</t>
+          <t>00:06:52</t>
         </is>
       </c>
       <c r="D41" s="10" t="inlineStr">
         <is>
-          <t>2021-12-20T14:16:50Z</t>
+          <t>2021-12-26T05:53:57Z</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="12" t="inlineStr">
         <is>
-          <t>037 Loops</t>
+          <t>039 impl blocks</t>
         </is>
       </c>
       <c r="B42" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=11yZ9n7m0uU</t>
+          <t>https://www.youtube.com/watch?v=rsVasi_rchU</t>
         </is>
       </c>
       <c r="C42" s="14" t="inlineStr">
         <is>
-          <t>00:06:42</t>
+          <t>00:08:57</t>
         </is>
       </c>
       <c r="D42" s="10" t="inlineStr">
         <is>
-          <t>2021-12-25T04:29:15Z</t>
+          <t>2021-12-26T05:55:58Z</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="12" t="inlineStr">
         <is>
-          <t>038 More loops</t>
+          <t>040 More impl blocks</t>
         </is>
       </c>
       <c r="B43" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=1xhe1eQRKsk</t>
+          <t>https://www.youtube.com/watch?v=x34LmxDa76Y</t>
         </is>
       </c>
       <c r="C43" s="14" t="inlineStr">
         <is>
-          <t>00:06:52</t>
+          <t>00:08:54</t>
         </is>
       </c>
       <c r="D43" s="10" t="inlineStr">
         <is>
-          <t>2021-12-26T05:53:57Z</t>
+          <t>2021-12-26T05:58:29Z</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="12" t="inlineStr">
         <is>
-          <t>039 impl blocks</t>
+          <t>041 enum impl blocks</t>
         </is>
       </c>
       <c r="B44" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=rsVasi_rchU</t>
+          <t>https://www.youtube.com/watch?v=DJJ_XsKNpZk</t>
         </is>
       </c>
       <c r="C44" s="14" t="inlineStr">
         <is>
-          <t>00:08:57</t>
+          <t>00:10:27</t>
         </is>
       </c>
       <c r="D44" s="10" t="inlineStr">
         <is>
-          <t>2021-12-26T05:55:58Z</t>
+          <t>2021-12-26T06:00:29Z</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="12" t="inlineStr">
         <is>
-          <t>040 More impl blocks</t>
+          <t>042 More destructuring</t>
         </is>
       </c>
       <c r="B45" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=x34LmxDa76Y</t>
+          <t>https://www.youtube.com/watch?v=HtR8vPWmeGs</t>
         </is>
       </c>
       <c r="C45" s="14" t="inlineStr">
         <is>
-          <t>00:08:54</t>
+          <t>00:09:46</t>
         </is>
       </c>
       <c r="D45" s="10" t="inlineStr">
         <is>
-          <t>2021-12-26T05:58:29Z</t>
+          <t>2021-12-26T06:01:58Z</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="12" t="inlineStr">
         <is>
-          <t>041 enum impl blocks</t>
+          <t>043 Dereferencing and the dot operator</t>
         </is>
       </c>
       <c r="B46" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=DJJ_XsKNpZk</t>
+          <t>https://www.youtube.com/watch?v=znCUAqyfbe4</t>
         </is>
       </c>
       <c r="C46" s="14" t="inlineStr">
         <is>
-          <t>00:10:27</t>
+          <t>00:09:38</t>
         </is>
       </c>
       <c r="D46" s="10" t="inlineStr">
         <is>
-          <t>2021-12-26T06:00:29Z</t>
+          <t>2021-12-26T06:03:27Z</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="12" t="inlineStr">
         <is>
-          <t>042 More destructuring</t>
+          <t>044 Generics</t>
         </is>
       </c>
       <c r="B47" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=HtR8vPWmeGs</t>
+          <t>https://www.youtube.com/watch?v=o4Hqyfjxtco</t>
         </is>
       </c>
       <c r="C47" s="14" t="inlineStr">
         <is>
-          <t>00:09:46</t>
+          <t>00:08:46</t>
         </is>
       </c>
       <c r="D47" s="10" t="inlineStr">
         <is>
-          <t>2021-12-26T06:01:58Z</t>
+          <t>2022-01-01T05:17:35Z</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="12" t="inlineStr">
         <is>
-          <t>043 Dereferencing and the dot operator</t>
+          <t>045 More generics</t>
         </is>
       </c>
       <c r="B48" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=znCUAqyfbe4</t>
+          <t>https://www.youtube.com/watch?v=yqJowwt2JIU</t>
         </is>
       </c>
       <c r="C48" s="14" t="inlineStr">
         <is>
-          <t>00:09:38</t>
+          <t>00:07:33</t>
         </is>
       </c>
       <c r="D48" s="10" t="inlineStr">
         <is>
-          <t>2021-12-26T06:03:27Z</t>
+          <t>2022-01-02T03:47:47Z</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="12" t="inlineStr">
         <is>
-          <t>044 Generics</t>
+          <t>046 Option</t>
         </is>
       </c>
       <c r="B49" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=o4Hqyfjxtco</t>
+          <t>https://www.youtube.com/watch?v=Or-ju7nvN58</t>
         </is>
       </c>
       <c r="C49" s="14" t="inlineStr">
         <is>
-          <t>00:08:46</t>
+          <t>00:08:04</t>
         </is>
       </c>
       <c r="D49" s="10" t="inlineStr">
         <is>
-          <t>2022-01-01T05:17:35Z</t>
+          <t>2022-01-03T03:56:13Z</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="12" t="inlineStr">
         <is>
-          <t>045 More generics</t>
+          <t>047 More Option</t>
         </is>
       </c>
       <c r="B50" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=yqJowwt2JIU</t>
+          <t>https://www.youtube.com/watch?v=uhMO2b13bUA</t>
         </is>
       </c>
       <c r="C50" s="14" t="inlineStr">
         <is>
-          <t>00:07:33</t>
+          <t>00:07:31</t>
         </is>
       </c>
       <c r="D50" s="10" t="inlineStr">
         <is>
-          <t>2022-01-02T03:47:47Z</t>
+          <t>2022-01-03T03:57:35Z</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="12" t="inlineStr">
         <is>
-          <t>046 Option</t>
+          <t>048 Result</t>
         </is>
       </c>
       <c r="B51" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=Or-ju7nvN58</t>
+          <t>https://www.youtube.com/watch?v=ijWLXEsW7dY</t>
         </is>
       </c>
       <c r="C51" s="14" t="inlineStr">
         <is>
-          <t>00:08:04</t>
+          <t>00:08:49</t>
         </is>
       </c>
       <c r="D51" s="10" t="inlineStr">
         <is>
-          <t>2022-01-03T03:56:13Z</t>
+          <t>2022-01-05T00:12:48Z</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="12" t="inlineStr">
         <is>
-          <t>047 More Option</t>
+          <t>049 More Result</t>
         </is>
       </c>
       <c r="B52" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=uhMO2b13bUA</t>
+          <t>https://www.youtube.com/watch?v=js3CR_cszOM</t>
         </is>
       </c>
       <c r="C52" s="14" t="inlineStr">
         <is>
-          <t>00:07:31</t>
+          <t>00:11:35</t>
         </is>
       </c>
       <c r="D52" s="10" t="inlineStr">
         <is>
-          <t>2022-01-03T03:57:35Z</t>
+          <t>2022-01-06T04:34:17Z</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="12" t="inlineStr">
         <is>
-          <t>048 Result</t>
+          <t>050 if let and while let</t>
         </is>
       </c>
       <c r="B53" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=ijWLXEsW7dY</t>
+          <t>https://www.youtube.com/watch?v=VYFOnb4VJ5Y</t>
         </is>
       </c>
       <c r="C53" s="14" t="inlineStr">
         <is>
-          <t>00:08:49</t>
+          <t>00:13:25</t>
         </is>
       </c>
       <c r="D53" s="10" t="inlineStr">
         <is>
-          <t>2022-01-05T00:12:48Z</t>
+          <t>2022-01-06T04:35:37Z</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="12" t="inlineStr">
         <is>
-          <t>049 More Result</t>
+          <t>051 HashMap and BTreeMap</t>
         </is>
       </c>
       <c r="B54" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=js3CR_cszOM</t>
+          <t>https://www.youtube.com/watch?v=NvaDxXZMWNk</t>
         </is>
       </c>
       <c r="C54" s="14" t="inlineStr">
         <is>
-          <t>00:11:35</t>
+          <t>00:08:40</t>
         </is>
       </c>
       <c r="D54" s="10" t="inlineStr">
         <is>
-          <t>2022-01-06T04:34:17Z</t>
+          <t>2022-01-08T05:53:16Z</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="12" t="inlineStr">
         <is>
-          <t>050 if let and while let</t>
+          <t>052 More HashMap</t>
         </is>
       </c>
       <c r="B55" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=VYFOnb4VJ5Y</t>
+          <t>https://www.youtube.com/watch?v=NBD0kmaOPro</t>
         </is>
       </c>
       <c r="C55" s="14" t="inlineStr">
         <is>
-          <t>00:13:25</t>
+          <t>00:09:15</t>
         </is>
       </c>
       <c r="D55" s="10" t="inlineStr">
         <is>
-          <t>2022-01-06T04:35:37Z</t>
+          <t>2022-01-08T15:18:32Z</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="12" t="inlineStr">
         <is>
-          <t>051 HashMap and BTreeMap</t>
+          <t>053 HashMap entry method</t>
         </is>
       </c>
       <c r="B56" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=NvaDxXZMWNk</t>
+          <t>https://www.youtube.com/watch?v=piK3ySJZpdA</t>
         </is>
       </c>
       <c r="C56" s="14" t="inlineStr">
         <is>
-          <t>00:08:40</t>
+          <t>00:11:23</t>
         </is>
       </c>
       <c r="D56" s="10" t="inlineStr">
         <is>
-          <t>2022-01-08T05:53:16Z</t>
+          <t>2022-01-08T15:21:22Z</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="12" t="inlineStr">
         <is>
-          <t>052 More HashMap</t>
+          <t>054 HashMap entry and HashSet</t>
         </is>
       </c>
       <c r="B57" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=NBD0kmaOPro</t>
+          <t>https://www.youtube.com/watch?v=Tea69-G7ER8</t>
         </is>
       </c>
       <c r="C57" s="14" t="inlineStr">
         <is>
-          <t>00:09:15</t>
+          <t>00:12:23</t>
         </is>
       </c>
       <c r="D57" s="10" t="inlineStr">
         <is>
-          <t>2022-01-08T15:18:32Z</t>
+          <t>2022-01-08T15:23:03Z</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="12" t="inlineStr">
         <is>
-          <t>053 HashMap entry method</t>
+          <t>055 BinaryHeap</t>
         </is>
       </c>
       <c r="B58" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=piK3ySJZpdA</t>
+          <t>https://www.youtube.com/watch?v=DAlSUUfaevs</t>
         </is>
       </c>
       <c r="C58" s="14" t="inlineStr">
         <is>
-          <t>00:11:23</t>
+          <t>00:08:52</t>
         </is>
       </c>
       <c r="D58" s="10" t="inlineStr">
         <is>
-          <t>2022-01-08T15:21:22Z</t>
+          <t>2022-01-08T15:24:47Z</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="12" t="inlineStr">
         <is>
-          <t>054 HashMap entry and HashSet</t>
+          <t>056 VecDeque</t>
         </is>
       </c>
       <c r="B59" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=Tea69-G7ER8</t>
+          <t>https://www.youtube.com/watch?v=vM42cJIwjbE</t>
         </is>
       </c>
       <c r="C59" s="14" t="inlineStr">
         <is>
-          <t>00:12:23</t>
+          <t>00:07:34</t>
         </is>
       </c>
       <c r="D59" s="10" t="inlineStr">
         <is>
-          <t>2022-01-08T15:23:03Z</t>
+          <t>2022-01-08T15:26:57Z</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="12" t="inlineStr">
         <is>
-          <t>055 BinaryHeap</t>
+          <t>057 Question mark operator</t>
         </is>
       </c>
       <c r="B60" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=DAlSUUfaevs</t>
+          <t>https://www.youtube.com/watch?v=rkMQk7wmXKk</t>
         </is>
       </c>
       <c r="C60" s="14" t="inlineStr">
         <is>
-          <t>00:08:52</t>
+          <t>00:11:17</t>
         </is>
       </c>
       <c r="D60" s="10" t="inlineStr">
         <is>
-          <t>2022-01-08T15:24:47Z</t>
+          <t>2022-01-08T15:28:56Z</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="12" t="inlineStr">
         <is>
-          <t>056 VecDeque</t>
+          <t>058 Formatting news!</t>
         </is>
       </c>
       <c r="B61" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=vM42cJIwjbE</t>
+          <t>https://www.youtube.com/watch?v=l5f3U5nZR7w</t>
         </is>
       </c>
       <c r="C61" s="14" t="inlineStr">
         <is>
-          <t>00:07:34</t>
+          <t>00:08:40</t>
         </is>
       </c>
       <c r="D61" s="10" t="inlineStr">
         <is>
-          <t>2022-01-08T15:26:57Z</t>
+          <t>2022-01-15T06:11:13Z</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="12" t="inlineStr">
         <is>
-          <t>057 Question mark operator</t>
+          <t>059 Trait intro</t>
         </is>
       </c>
       <c r="B62" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=rkMQk7wmXKk</t>
+          <t>https://www.youtube.com/watch?v=xE2Ixd1A5Sc</t>
         </is>
       </c>
       <c r="C62" s="14" t="inlineStr">
         <is>
-          <t>00:11:17</t>
+          <t>00:08:39</t>
         </is>
       </c>
       <c r="D62" s="10" t="inlineStr">
         <is>
-          <t>2022-01-08T15:28:56Z</t>
+          <t>2022-01-15T07:01:03Z</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="12" t="inlineStr">
         <is>
-          <t>058 Formatting news!</t>
+          <t>060 A simple trait</t>
         </is>
       </c>
       <c r="B63" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=l5f3U5nZR7w</t>
+          <t>https://www.youtube.com/watch?v=BiYdPeDyeeE</t>
         </is>
       </c>
       <c r="C63" s="14" t="inlineStr">
         <is>
-          <t>00:08:40</t>
+          <t>00:06:22</t>
         </is>
       </c>
       <c r="D63" s="10" t="inlineStr">
         <is>
-          <t>2022-01-15T06:11:13Z</t>
+          <t>2022-01-15T07:02:29Z</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="12" t="inlineStr">
         <is>
-          <t>059 Trait intro</t>
+          <t>061 Implementing a trait</t>
         </is>
       </c>
       <c r="B64" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=xE2Ixd1A5Sc</t>
+          <t>https://www.youtube.com/watch?v=qkwmw-HWysU</t>
         </is>
       </c>
       <c r="C64" s="14" t="inlineStr">
         <is>
-          <t>00:08:39</t>
+          <t>00:09:24</t>
         </is>
       </c>
       <c r="D64" s="10" t="inlineStr">
         <is>
-          <t>2022-01-15T07:01:03Z</t>
+          <t>2022-01-15T07:04:47Z</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="12" t="inlineStr">
         <is>
-          <t>060 A simple trait</t>
+          <t>062 Another small trait</t>
         </is>
       </c>
       <c r="B65" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=BiYdPeDyeeE</t>
+          <t>https://www.youtube.com/watch?v=QdHqFooQSKg</t>
         </is>
       </c>
       <c r="C65" s="14" t="inlineStr">
         <is>
-          <t>00:06:22</t>
+          <t>00:10:17</t>
         </is>
       </c>
       <c r="D65" s="10" t="inlineStr">
         <is>
-          <t>2022-01-15T07:02:29Z</t>
+          <t>2022-01-15T07:06:12Z</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="12" t="inlineStr">
         <is>
-          <t>061 Implementing a trait</t>
+          <t>063 Traits as bounds</t>
         </is>
       </c>
       <c r="B66" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=qkwmw-HWysU</t>
+          <t>https://www.youtube.com/watch?v=zILeN_EMqU0</t>
         </is>
       </c>
       <c r="C66" s="14" t="inlineStr">
         <is>
-          <t>00:09:24</t>
+          <t>00:10:06</t>
         </is>
       </c>
       <c r="D66" s="10" t="inlineStr">
         <is>
-          <t>2022-01-15T07:04:47Z</t>
+          <t>2022-01-15T07:07:59Z</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="12" t="inlineStr">
         <is>
-          <t>062 Another small trait</t>
+          <t>064 Implementing From</t>
         </is>
       </c>
       <c r="B67" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=QdHqFooQSKg</t>
+          <t>https://www.youtube.com/watch?v=FMyVR_pqU7A</t>
         </is>
       </c>
       <c r="C67" s="14" t="inlineStr">
         <is>
-          <t>00:10:17</t>
+          <t>00:12:47</t>
         </is>
       </c>
       <c r="D67" s="10" t="inlineStr">
         <is>
-          <t>2022-01-15T07:06:12Z</t>
+          <t>2022-01-15T07:09:19Z</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="12" t="inlineStr">
         <is>
-          <t>063 Traits as bounds</t>
+          <t>065 Blanket trait implementations</t>
         </is>
       </c>
       <c r="B68" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=zILeN_EMqU0</t>
+          <t>https://www.youtube.com/watch?v=ggUcYGxQYWY</t>
         </is>
       </c>
       <c r="C68" s="14" t="inlineStr">
         <is>
-          <t>00:10:06</t>
+          <t>00:11:51</t>
         </is>
       </c>
       <c r="D68" s="10" t="inlineStr">
         <is>
-          <t>2022-01-15T07:07:59Z</t>
+          <t>2022-01-22T06:35:02Z</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="12" t="inlineStr">
         <is>
-          <t>064 Implementing From</t>
+          <t>066 Getting ToString for free</t>
         </is>
       </c>
       <c r="B69" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=FMyVR_pqU7A</t>
+          <t>https://www.youtube.com/watch?v=VeeXoHYkQPI</t>
         </is>
       </c>
       <c r="C69" s="14" t="inlineStr">
         <is>
-          <t>00:12:47</t>
+          <t>00:04:27</t>
         </is>
       </c>
       <c r="D69" s="10" t="inlineStr">
         <is>
-          <t>2022-01-15T07:09:19Z</t>
+          <t>2022-01-22T06:38:19Z</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="12" t="inlineStr">
         <is>
-          <t>065 Blanket trait implementations</t>
+          <t>067 The AsRef trait</t>
         </is>
       </c>
       <c r="B70" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=ggUcYGxQYWY</t>
+          <t>https://www.youtube.com/watch?v=A0ZLHnCSO3k</t>
         </is>
       </c>
       <c r="C70" s="14" t="inlineStr">
         <is>
-          <t>00:11:51</t>
+          <t>00:05:06</t>
         </is>
       </c>
       <c r="D70" s="10" t="inlineStr">
         <is>
-          <t>2022-01-22T06:35:02Z</t>
+          <t>2022-01-22T06:41:38Z</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="12" t="inlineStr">
         <is>
-          <t>066 Getting ToString for free</t>
+          <t>068 Chaining methods</t>
         </is>
       </c>
       <c r="B71" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=VeeXoHYkQPI</t>
+          <t>https://www.youtube.com/watch?v=I05kBKMvpz0</t>
         </is>
       </c>
       <c r="C71" s="14" t="inlineStr">
         <is>
-          <t>00:04:27</t>
+          <t>00:08:05</t>
         </is>
       </c>
       <c r="D71" s="10" t="inlineStr">
         <is>
-          <t>2022-01-22T06:38:19Z</t>
+          <t>2022-01-22T06:44:07Z</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="12" t="inlineStr">
         <is>
-          <t>067 The AsRef trait</t>
+          <t>069 Iterator intro</t>
         </is>
       </c>
       <c r="B72" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=A0ZLHnCSO3k</t>
+          <t>https://www.youtube.com/watch?v=uHzakmeaVL8</t>
         </is>
       </c>
       <c r="C72" s="14" t="inlineStr">
         <is>
-          <t>00:05:06</t>
+          <t>00:08:46</t>
         </is>
       </c>
       <c r="D72" s="10" t="inlineStr">
         <is>
-          <t>2022-01-22T06:41:38Z</t>
+          <t>2022-01-22T06:47:04Z</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="12" t="inlineStr">
         <is>
-          <t>068 Chaining methods</t>
+          <t>070 Iterators and assert_eq!</t>
         </is>
       </c>
       <c r="B73" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=I05kBKMvpz0</t>
+          <t>https://www.youtube.com/watch?v=50mrYgeXg3s</t>
         </is>
       </c>
       <c r="C73" s="14" t="inlineStr">
         <is>
-          <t>00:08:05</t>
+          <t>00:08:50</t>
         </is>
       </c>
       <c r="D73" s="10" t="inlineStr">
         <is>
-          <t>2022-01-22T06:44:07Z</t>
+          <t>2022-01-22T06:49:53Z</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="12" t="inlineStr">
         <is>
-          <t>069 Iterator intro</t>
+          <t>071 Implementing Iterator</t>
         </is>
       </c>
       <c r="B74" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=uHzakmeaVL8</t>
+          <t>https://www.youtube.com/watch?v=5N046GJ4tMI</t>
         </is>
       </c>
       <c r="C74" s="14" t="inlineStr">
         <is>
-          <t>00:08:46</t>
+          <t>00:09:46</t>
         </is>
       </c>
       <c r="D74" s="10" t="inlineStr">
         <is>
-          <t>2022-01-22T06:47:04Z</t>
+          <t>2022-01-22T06:52:58Z</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="12" t="inlineStr">
         <is>
-          <t>070 Iterators and assert_eq!</t>
+          <t>072 Intro to closures</t>
         </is>
       </c>
       <c r="B75" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=50mrYgeXg3s</t>
+          <t>https://www.youtube.com/watch?v=NJnLPaX7UOs</t>
         </is>
       </c>
       <c r="C75" s="14" t="inlineStr">
         <is>
-          <t>00:08:50</t>
+          <t>00:09:56</t>
         </is>
       </c>
       <c r="D75" s="10" t="inlineStr">
         <is>
-          <t>2022-01-22T06:49:53Z</t>
+          <t>2022-01-29T05:14:27Z</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="12" t="inlineStr">
         <is>
-          <t>071 Implementing Iterator</t>
+          <t>073 Zero cost abstractions</t>
         </is>
       </c>
       <c r="B76" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=5N046GJ4tMI</t>
+          <t>https://www.youtube.com/watch?v=Htn-mwpw0lk</t>
         </is>
       </c>
       <c r="C76" s="14" t="inlineStr">
         <is>
-          <t>00:09:46</t>
+          <t>00:08:37</t>
         </is>
       </c>
       <c r="D76" s="10" t="inlineStr">
         <is>
-          <t>2022-01-22T06:52:58Z</t>
+          <t>2022-01-29T06:09:21Z</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="12" t="inlineStr">
         <is>
-          <t>072 Intro to closures</t>
+          <t>074 map and for_each</t>
         </is>
       </c>
       <c r="B77" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=NJnLPaX7UOs</t>
+          <t>https://www.youtube.com/watch?v=fcRTIhysVFQ</t>
         </is>
       </c>
       <c r="C77" s="14" t="inlineStr">
         <is>
-          <t>00:09:56</t>
+          <t>00:08:15</t>
         </is>
       </c>
       <c r="D77" s="10" t="inlineStr">
         <is>
-          <t>2022-01-29T05:14:27Z</t>
+          <t>2022-01-29T06:13:16Z</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="12" t="inlineStr">
         <is>
-          <t>073 Zero cost abstractions</t>
+          <t>075 zipping iterators</t>
         </is>
       </c>
       <c r="B78" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=Htn-mwpw0lk</t>
+          <t>https://www.youtube.com/watch?v=AOu9ZGi6O5U</t>
         </is>
       </c>
       <c r="C78" s="14" t="inlineStr">
         <is>
-          <t>00:08:37</t>
+          <t>00:10:42</t>
         </is>
       </c>
       <c r="D78" s="10" t="inlineStr">
         <is>
-          <t>2022-01-29T06:09:21Z</t>
+          <t>2022-01-29T06:15:31Z</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="12" t="inlineStr">
         <is>
-          <t>074 map and for_each</t>
+          <t>076 char methods</t>
         </is>
       </c>
       <c r="B79" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=fcRTIhysVFQ</t>
+          <t>https://www.youtube.com/watch?v=y8Lz6vvzpsY</t>
         </is>
       </c>
       <c r="C79" s="14" t="inlineStr">
         <is>
-          <t>00:08:15</t>
+          <t>00:08:24</t>
         </is>
       </c>
       <c r="D79" s="10" t="inlineStr">
         <is>
-          <t>2022-01-29T06:13:16Z</t>
+          <t>2022-01-29T06:18:24Z</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="12" t="inlineStr">
         <is>
-          <t>075 zipping iterators</t>
+          <t>077 filter, filter_map</t>
         </is>
       </c>
       <c r="B80" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=AOu9ZGi6O5U</t>
+          <t>https://www.youtube.com/watch?v=RgnTv-LklDg</t>
         </is>
       </c>
       <c r="C80" s="14" t="inlineStr">
         <is>
-          <t>00:10:42</t>
+          <t>00:12:19</t>
         </is>
       </c>
       <c r="D80" s="10" t="inlineStr">
         <is>
-          <t>2022-01-29T06:15:31Z</t>
+          <t>2022-01-29T06:20:34Z</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="12" t="inlineStr">
         <is>
-          <t>076 char methods</t>
+          <t>078 ok_or, ok_or_else</t>
         </is>
       </c>
       <c r="B81" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=y8Lz6vvzpsY</t>
+          <t>https://www.youtube.com/watch?v=revoQGNW9a0</t>
         </is>
       </c>
       <c r="C81" s="14" t="inlineStr">
         <is>
-          <t>00:08:24</t>
+          <t>00:13:25</t>
         </is>
       </c>
       <c r="D81" s="10" t="inlineStr">
         <is>
-          <t>2022-01-29T06:18:24Z</t>
+          <t>2022-01-29T06:22:34Z</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="12" t="inlineStr">
         <is>
-          <t>077 filter, filter_map</t>
+          <t>079 map, and_then for Option</t>
         </is>
       </c>
       <c r="B82" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=RgnTv-LklDg</t>
+          <t>https://www.youtube.com/watch?v=qWJtCljWA58</t>
         </is>
       </c>
       <c r="C82" s="14" t="inlineStr">
         <is>
-          <t>00:12:19</t>
+          <t>00:09:47</t>
         </is>
       </c>
       <c r="D82" s="10" t="inlineStr">
         <is>
-          <t>2022-01-29T06:20:34Z</t>
+          <t>2022-02-05T06:49:12Z</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="12" t="inlineStr">
         <is>
-          <t>078 ok_or, ok_or_else</t>
+          <t>080 and, or for Option</t>
         </is>
       </c>
       <c r="B83" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=revoQGNW9a0</t>
+          <t>https://www.youtube.com/watch?v=zngFHGftPdM</t>
         </is>
       </c>
       <c r="C83" s="14" t="inlineStr">
         <is>
-          <t>00:13:25</t>
+          <t>00:08:35</t>
         </is>
       </c>
       <c r="D83" s="10" t="inlineStr">
         <is>
-          <t>2022-01-29T06:22:34Z</t>
+          <t>2022-02-05T06:57:02Z</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="12" t="inlineStr">
         <is>
-          <t>079 map, and_then for Option</t>
+          <t>081 any, all methods</t>
         </is>
       </c>
       <c r="B84" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=qWJtCljWA58</t>
+          <t>https://www.youtube.com/watch?v=koxer6Fg-as</t>
         </is>
       </c>
       <c r="C84" s="14" t="inlineStr">
         <is>
-          <t>00:09:47</t>
+          <t>00:10:43</t>
         </is>
       </c>
       <c r="D84" s="10" t="inlineStr">
         <is>
-          <t>2022-02-05T06:49:12Z</t>
+          <t>2022-02-05T07:00:04Z</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="12" t="inlineStr">
         <is>
-          <t>080 and, or for Option</t>
+          <t>082 reverse iterators</t>
         </is>
       </c>
       <c r="B85" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=zngFHGftPdM</t>
+          <t>https://www.youtube.com/watch?v=TC5hK511fg0</t>
         </is>
       </c>
       <c r="C85" s="14" t="inlineStr">
         <is>
-          <t>00:08:35</t>
+          <t>00:07:17</t>
         </is>
       </c>
       <c r="D85" s="10" t="inlineStr">
         <is>
-          <t>2022-02-05T06:57:02Z</t>
+          <t>2022-02-05T07:02:12Z</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="12" t="inlineStr">
         <is>
-          <t>081 any, all methods</t>
+          <t>083 find, position, cycle</t>
         </is>
       </c>
       <c r="B86" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=koxer6Fg-as</t>
+          <t>https://www.youtube.com/watch?v=CrvDhk1miLE</t>
         </is>
       </c>
       <c r="C86" s="14" t="inlineStr">
         <is>
-          <t>00:10:43</t>
+          <t>00:10:15</t>
         </is>
       </c>
       <c r="D86" s="10" t="inlineStr">
         <is>
-          <t>2022-02-05T07:00:04Z</t>
+          <t>2022-02-05T07:05:04Z</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="12" t="inlineStr">
         <is>
-          <t>082 reverse iterators</t>
+          <t>084 skip, fold methods</t>
         </is>
       </c>
       <c r="B87" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=TC5hK511fg0</t>
+          <t>https://www.youtube.com/watch?v=LNfhXppiiW8</t>
         </is>
       </c>
       <c r="C87" s="14" t="inlineStr">
         <is>
-          <t>00:07:17</t>
+          <t>00:10:26</t>
         </is>
       </c>
       <c r="D87" s="10" t="inlineStr">
         <is>
-          <t>2022-02-05T07:02:12Z</t>
+          <t>2022-02-05T07:11:23Z</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="12" t="inlineStr">
         <is>
-          <t>083 find, position, cycle</t>
+          <t>085 fold method again</t>
         </is>
       </c>
       <c r="B88" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=CrvDhk1miLE</t>
+          <t>https://www.youtube.com/watch?v=lG651CzNFmM</t>
         </is>
       </c>
       <c r="C88" s="14" t="inlineStr">
         <is>
-          <t>00:10:15</t>
+          <t>00:07:35</t>
         </is>
       </c>
       <c r="D88" s="10" t="inlineStr">
         <is>
-          <t>2022-02-05T07:05:04Z</t>
+          <t>2022-02-05T07:13:35Z</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="12" t="inlineStr">
         <is>
-          <t>084 skip, fold methods</t>
+          <t>086 chunks, windows</t>
         </is>
       </c>
       <c r="B89" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=LNfhXppiiW8</t>
+          <t>https://www.youtube.com/watch?v=k7M79aEbUWA</t>
         </is>
       </c>
       <c r="C89" s="14" t="inlineStr">
         <is>
-          <t>00:10:26</t>
+          <t>00:10:50</t>
         </is>
       </c>
       <c r="D89" s="10" t="inlineStr">
         <is>
-          <t>2022-02-05T07:11:23Z</t>
+          <t>2022-02-12T06:10:20Z</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="12" t="inlineStr">
         <is>
-          <t>085 fold method again</t>
+          <t>087 match_indices, peekable</t>
         </is>
       </c>
       <c r="B90" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=lG651CzNFmM</t>
+          <t>https://www.youtube.com/watch?v=PPkOsAoCatw</t>
         </is>
       </c>
       <c r="C90" s="14" t="inlineStr">
         <is>
-          <t>00:07:35</t>
+          <t>00:08:06</t>
         </is>
       </c>
       <c r="D90" s="10" t="inlineStr">
         <is>
-          <t>2022-02-05T07:13:35Z</t>
+          <t>2022-02-12T06:40:01Z</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="12" t="inlineStr">
         <is>
-          <t>086 chunks, windows</t>
+          <t>088 the dbg! macro</t>
         </is>
       </c>
       <c r="B91" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=k7M79aEbUWA</t>
+          <t>https://www.youtube.com/watch?v=69K62zawGwA</t>
         </is>
       </c>
       <c r="C91" s="14" t="inlineStr">
         <is>
-          <t>00:10:50</t>
+          <t>00:08:54</t>
         </is>
       </c>
       <c r="D91" s="10" t="inlineStr">
         <is>
-          <t>2022-02-12T06:10:20Z</t>
+          <t>2022-02-12T06:42:39Z</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="12" t="inlineStr">
         <is>
-          <t>087 match_indices, peekable</t>
+          <t>089 Inspect, String and &amp;str</t>
         </is>
       </c>
       <c r="B92" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=PPkOsAoCatw</t>
+          <t>https://www.youtube.com/watch?v=kG6shBpcGkU</t>
         </is>
       </c>
       <c r="C92" s="14" t="inlineStr">
         <is>
-          <t>00:08:06</t>
+          <t>00:10:33</t>
         </is>
       </c>
       <c r="D92" s="10" t="inlineStr">
         <is>
-          <t>2022-02-12T06:40:01Z</t>
+          <t>2022-02-12T06:46:35Z</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="12" t="inlineStr">
         <is>
-          <t>088 the dbg! macro</t>
+          <t>090 Lifetimes intro</t>
         </is>
       </c>
       <c r="B93" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=69K62zawGwA</t>
+          <t>https://www.youtube.com/watch?v=zwKC3Gau5jY</t>
         </is>
       </c>
       <c r="C93" s="14" t="inlineStr">
         <is>
-          <t>00:08:54</t>
+          <t>00:11:09</t>
         </is>
       </c>
       <c r="D93" s="10" t="inlineStr">
         <is>
-          <t>2022-02-12T06:42:39Z</t>
+          <t>2022-02-12T06:50:49Z</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="12" t="inlineStr">
         <is>
-          <t>089 Inspect, String and &amp;str</t>
+          <t>091 More lifetimes</t>
         </is>
       </c>
       <c r="B94" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=kG6shBpcGkU</t>
+          <t>https://www.youtube.com/watch?v=eYPQen8RiLY</t>
         </is>
       </c>
       <c r="C94" s="14" t="inlineStr">
         <is>
-          <t>00:10:33</t>
+          <t>00:11:57</t>
         </is>
       </c>
       <c r="D94" s="10" t="inlineStr">
         <is>
-          <t>2022-02-12T06:46:35Z</t>
+          <t>2022-02-12T06:52:27Z</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="12" t="inlineStr">
         <is>
-          <t>090 Lifetimes intro</t>
+          <t>092 Manual Debug impl</t>
         </is>
       </c>
       <c r="B95" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=zwKC3Gau5jY</t>
+          <t>https://www.youtube.com/watch?v=GX6Iecmk_kg</t>
         </is>
       </c>
       <c r="C95" s="14" t="inlineStr">
         <is>
-          <t>00:11:09</t>
+          <t>00:09:42</t>
         </is>
       </c>
       <c r="D95" s="10" t="inlineStr">
         <is>
-          <t>2022-02-12T06:50:49Z</t>
+          <t>2022-02-12T06:54:36Z</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="12" t="inlineStr">
         <is>
-          <t>091 More lifetimes</t>
+          <t>093 Interior mutability and Cell</t>
         </is>
       </c>
       <c r="B96" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=eYPQen8RiLY</t>
+          <t>https://www.youtube.com/watch?v=Bfqx_V2gp1Y</t>
         </is>
       </c>
       <c r="C96" s="14" t="inlineStr">
         <is>
-          <t>00:11:57</t>
+          <t>00:10:30</t>
         </is>
       </c>
       <c r="D96" s="10" t="inlineStr">
         <is>
-          <t>2022-02-12T06:52:27Z</t>
+          <t>2022-02-19T05:06:43Z</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="12" t="inlineStr">
         <is>
-          <t>092 Manual Debug impl</t>
+          <t>094 RefCell</t>
         </is>
       </c>
       <c r="B97" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=GX6Iecmk_kg</t>
+          <t>https://www.youtube.com/watch?v=-V-jCwGDTSk</t>
         </is>
       </c>
       <c r="C97" s="14" t="inlineStr">
         <is>
-          <t>00:09:42</t>
+          <t>00:11:18</t>
         </is>
       </c>
       <c r="D97" s="10" t="inlineStr">
         <is>
-          <t>2022-02-12T06:54:36Z</t>
+          <t>2022-02-19T05:08:22Z</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="12" t="inlineStr">
         <is>
-          <t>093 Interior mutability and Cell</t>
+          <t>095 RefCell again</t>
         </is>
       </c>
       <c r="B98" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=Bfqx_V2gp1Y</t>
+          <t>https://www.youtube.com/watch?v=-9aZWxM_GHY</t>
         </is>
       </c>
       <c r="C98" s="14" t="inlineStr">
         <is>
-          <t>00:10:30</t>
+          <t>00:09:32</t>
         </is>
       </c>
       <c r="D98" s="10" t="inlineStr">
         <is>
-          <t>2022-02-19T05:06:43Z</t>
+          <t>2022-02-20T06:01:05Z</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="12" t="inlineStr">
         <is>
-          <t>094 RefCell</t>
+          <t>096 Why interior mutability</t>
         </is>
       </c>
       <c r="B99" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=-V-jCwGDTSk</t>
+          <t>https://www.youtube.com/watch?v=pGNjiL223Zo</t>
         </is>
       </c>
       <c r="C99" s="14" t="inlineStr">
         <is>
-          <t>00:11:18</t>
+          <t>00:10:06</t>
         </is>
       </c>
       <c r="D99" s="10" t="inlineStr">
         <is>
-          <t>2022-02-19T05:08:22Z</t>
+          <t>2022-02-20T06:51:26Z</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="12" t="inlineStr">
         <is>
-          <t>095 RefCell again</t>
+          <t>097 Rc (reference counting)</t>
         </is>
       </c>
       <c r="B100" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=-9aZWxM_GHY</t>
+          <t>https://www.youtube.com/watch?v=Gm7Z6sp4Rk4</t>
         </is>
       </c>
       <c r="C100" s="14" t="inlineStr">
         <is>
-          <t>00:09:32</t>
+          <t>00:10:54</t>
         </is>
       </c>
       <c r="D100" s="10" t="inlineStr">
         <is>
-          <t>2022-02-20T06:01:05Z</t>
+          <t>2022-02-20T07:01:16Z</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="12" t="inlineStr">
         <is>
-          <t>096 Why interior mutability</t>
+          <t>098 Rc example</t>
         </is>
       </c>
       <c r="B101" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=pGNjiL223Zo</t>
+          <t>https://www.youtube.com/watch?v=F0TkBqUMSFU</t>
         </is>
       </c>
       <c r="C101" s="14" t="inlineStr">
         <is>
-          <t>00:10:06</t>
+          <t>00:09:58</t>
         </is>
       </c>
       <c r="D101" s="10" t="inlineStr">
         <is>
-          <t>2022-02-20T06:51:26Z</t>
+          <t>2022-02-20T07:05:46Z</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="12" t="inlineStr">
         <is>
-          <t>097 Rc (reference counting)</t>
+          <t>099 Rc and RefCell example</t>
         </is>
       </c>
       <c r="B102" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=Gm7Z6sp4Rk4</t>
+          <t>https://www.youtube.com/watch?v=2LmnrZvZ5Ns</t>
         </is>
       </c>
       <c r="C102" s="14" t="inlineStr">
         <is>
-          <t>00:10:54</t>
+          <t>00:09:33</t>
         </is>
       </c>
       <c r="D102" s="10" t="inlineStr">
         <is>
-          <t>2022-02-20T07:01:16Z</t>
+          <t>2022-02-20T07:08:55Z</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="12" t="inlineStr">
         <is>
-          <t>098 Rc example</t>
+          <t>100 Rust 1.59</t>
         </is>
       </c>
       <c r="B103" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=F0TkBqUMSFU</t>
+          <t>https://www.youtube.com/watch?v=hYt7Oj3tm00</t>
         </is>
       </c>
       <c r="C103" s="14" t="inlineStr">
         <is>
-          <t>00:09:58</t>
+          <t>00:15:10</t>
         </is>
       </c>
       <c r="D103" s="10" t="inlineStr">
         <is>
-          <t>2022-02-20T07:05:46Z</t>
+          <t>2022-02-26T07:24:46Z</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="12" t="inlineStr">
         <is>
-          <t>099 Rc and RefCell example</t>
+          <t>101 type alias and todo!() macro</t>
         </is>
       </c>
       <c r="B104" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=2LmnrZvZ5Ns</t>
+          <t>https://www.youtube.com/watch?v=maFEjLQQm40</t>
         </is>
       </c>
       <c r="C104" s="14" t="inlineStr">
         <is>
-          <t>00:09:33</t>
+          <t>00:08:39</t>
         </is>
       </c>
       <c r="D104" s="10" t="inlineStr">
         <is>
-          <t>2022-02-20T07:08:55Z</t>
+          <t>2022-02-26T07:53:53Z</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="12" t="inlineStr">
         <is>
-          <t>100 Rust 1.59</t>
+          <t>102 Cow</t>
         </is>
       </c>
       <c r="B105" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=hYt7Oj3tm00</t>
+          <t>https://www.youtube.com/watch?v=3HgcxuO_f8c</t>
         </is>
       </c>
       <c r="C105" s="14" t="inlineStr">
         <is>
-          <t>00:15:10</t>
+          <t>00:10:03</t>
         </is>
       </c>
       <c r="D105" s="10" t="inlineStr">
         <is>
-          <t>2022-02-26T07:24:46Z</t>
+          <t>2022-02-26T07:55:14Z</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="12" t="inlineStr">
         <is>
-          <t>101 type alias and todo!() macro</t>
+          <t>103 Multiple threads</t>
         </is>
       </c>
       <c r="B106" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=maFEjLQQm40</t>
+          <t>https://www.youtube.com/watch?v=iXR0wyTpBnY</t>
         </is>
       </c>
       <c r="C106" s="14" t="inlineStr">
         <is>
-          <t>00:08:39</t>
+          <t>00:11:16</t>
         </is>
       </c>
       <c r="D106" s="10" t="inlineStr">
         <is>
-          <t>2022-02-26T07:53:53Z</t>
+          <t>2022-02-26T08:02:53Z</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="12" t="inlineStr">
         <is>
-          <t>102 Cow</t>
+          <t>104 Mutex intro</t>
         </is>
       </c>
       <c r="B107" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=3HgcxuO_f8c</t>
+          <t>https://www.youtube.com/watch?v=3WaZPrxZYXw</t>
         </is>
       </c>
       <c r="C107" s="14" t="inlineStr">
         <is>
-          <t>00:10:03</t>
+          <t>00:10:25</t>
         </is>
       </c>
       <c r="D107" s="10" t="inlineStr">
         <is>
-          <t>2022-02-26T07:55:14Z</t>
+          <t>2022-02-26T08:05:15Z</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="12" t="inlineStr">
         <is>
-          <t>103 Multiple threads</t>
+          <t>105 Arc with Mutex</t>
         </is>
       </c>
       <c r="B108" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=iXR0wyTpBnY</t>
+          <t>https://www.youtube.com/watch?v=3MRpaICHaUs</t>
         </is>
       </c>
       <c r="C108" s="14" t="inlineStr">
         <is>
-          <t>00:11:16</t>
+          <t>00:09:13</t>
         </is>
       </c>
       <c r="D108" s="10" t="inlineStr">
         <is>
-          <t>2022-02-26T08:02:53Z</t>
+          <t>2022-02-26T08:06:43Z</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="12" t="inlineStr">
         <is>
-          <t>104 Mutex intro</t>
+          <t>106 Mutex and RwLock</t>
         </is>
       </c>
       <c r="B109" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=3WaZPrxZYXw</t>
+          <t>https://www.youtube.com/watch?v=11liIhj6jYg</t>
         </is>
       </c>
       <c r="C109" s="14" t="inlineStr">
         <is>
-          <t>00:10:25</t>
+          <t>00:09:46</t>
         </is>
       </c>
       <c r="D109" s="10" t="inlineStr">
         <is>
-          <t>2022-02-26T08:05:15Z</t>
+          <t>2022-02-26T08:07:48Z</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="12" t="inlineStr">
         <is>
-          <t>105 Arc with Mutex</t>
+          <t>107 Clippy</t>
         </is>
       </c>
       <c r="B110" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=3MRpaICHaUs</t>
+          <t>https://www.youtube.com/watch?v=LW_rfWf3G6k</t>
         </is>
       </c>
       <c r="C110" s="14" t="inlineStr">
         <is>
-          <t>00:09:13</t>
+          <t>00:11:20</t>
         </is>
       </c>
       <c r="D110" s="10" t="inlineStr">
         <is>
-          <t>2022-02-26T08:06:43Z</t>
+          <t>2022-03-05T09:15:17Z</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="12" t="inlineStr">
         <is>
-          <t>106 Mutex and RwLock</t>
+          <t>108 Box</t>
         </is>
       </c>
       <c r="B111" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=11liIhj6jYg</t>
+          <t>https://www.youtube.com/watch?v=NQ0cpno2VjU</t>
         </is>
       </c>
       <c r="C111" s="14" t="inlineStr">
         <is>
-          <t>00:09:46</t>
+          <t>00:08:30</t>
         </is>
       </c>
       <c r="D111" s="10" t="inlineStr">
         <is>
-          <t>2022-02-26T08:07:48Z</t>
+          <t>2022-03-05T09:22:06Z</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="12" t="inlineStr">
         <is>
-          <t>107 Clippy</t>
+          <t>109 Trait objects and Box</t>
         </is>
       </c>
       <c r="B112" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=LW_rfWf3G6k</t>
+          <t>https://www.youtube.com/watch?v=NIbIM2oT9bA</t>
         </is>
       </c>
       <c r="C112" s="14" t="inlineStr">
         <is>
-          <t>00:11:20</t>
+          <t>00:12:43</t>
         </is>
       </c>
       <c r="D112" s="10" t="inlineStr">
         <is>
-          <t>2022-03-05T09:15:17Z</t>
+          <t>2022-03-05T09:22:54Z</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="12" t="inlineStr">
         <is>
-          <t>108 Box</t>
+          <t>110 Three types of generics</t>
         </is>
       </c>
       <c r="B113" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=NQ0cpno2VjU</t>
+          <t>https://www.youtube.com/watch?v=sr9ief0b54Q</t>
         </is>
       </c>
       <c r="C113" s="14" t="inlineStr">
         <is>
-          <t>00:08:30</t>
+          <t>00:09:11</t>
         </is>
       </c>
       <c r="D113" s="10" t="inlineStr">
         <is>
-          <t>2022-03-05T09:22:06Z</t>
+          <t>2022-03-05T09:25:04Z</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="12" t="inlineStr">
         <is>
-          <t>109 Trait objects and Box</t>
+          <t>111 Function pointers</t>
         </is>
       </c>
       <c r="B114" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=NIbIM2oT9bA</t>
+          <t>https://www.youtube.com/watch?v=MV4DgEURRJg</t>
         </is>
       </c>
       <c r="C114" s="14" t="inlineStr">
         <is>
-          <t>00:12:43</t>
+          <t>00:08:22</t>
         </is>
       </c>
       <c r="D114" s="10" t="inlineStr">
         <is>
-          <t>2022-03-05T09:22:54Z</t>
+          <t>2022-03-05T09:26:30Z</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="12" t="inlineStr">
         <is>
-          <t>110 Three types of generics</t>
+          <t>112 Fn, FnMut, FnOnce</t>
         </is>
       </c>
       <c r="B115" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=sr9ief0b54Q</t>
+          <t>https://www.youtube.com/watch?v=AgdvKjUJodc</t>
         </is>
       </c>
       <c r="C115" s="14" t="inlineStr">
         <is>
-          <t>00:09:11</t>
+          <t>00:10:53</t>
         </is>
       </c>
       <c r="D115" s="10" t="inlineStr">
         <is>
-          <t>2022-03-05T09:25:04Z</t>
+          <t>2022-03-05T09:27:57Z</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="12" t="inlineStr">
         <is>
-          <t>111 Function pointers</t>
+          <t>113 About impl Trait</t>
         </is>
       </c>
       <c r="B116" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=MV4DgEURRJg</t>
+          <t>https://www.youtube.com/watch?v=C2dcFfNhEfc</t>
         </is>
       </c>
       <c r="C116" s="14" t="inlineStr">
         <is>
-          <t>00:08:22</t>
+          <t>00:09:18</t>
         </is>
       </c>
       <c r="D116" s="10" t="inlineStr">
         <is>
-          <t>2022-03-05T09:26:30Z</t>
+          <t>2022-03-05T09:29:17Z</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="12" t="inlineStr">
         <is>
-          <t>112 Fn, FnMut, FnOnce</t>
+          <t>114 Attributes part 1</t>
         </is>
       </c>
       <c r="B117" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=AgdvKjUJodc</t>
+          <t>https://www.youtube.com/watch?v=uvJGGBhBfgI</t>
         </is>
       </c>
       <c r="C117" s="14" t="inlineStr">
         <is>
-          <t>00:10:53</t>
+          <t>00:09:36</t>
         </is>
       </c>
       <c r="D117" s="10" t="inlineStr">
         <is>
-          <t>2022-03-05T09:27:57Z</t>
+          <t>2022-03-12T08:12:08Z</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="12" t="inlineStr">
         <is>
-          <t>113 About impl Trait</t>
+          <t>115 Attributes part 2</t>
         </is>
       </c>
       <c r="B118" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=C2dcFfNhEfc</t>
+          <t>https://www.youtube.com/watch?v=s1A84oJCp20</t>
         </is>
       </c>
       <c r="C118" s="14" t="inlineStr">
         <is>
-          <t>00:09:18</t>
+          <t>00:11:07</t>
         </is>
       </c>
       <c r="D118" s="10" t="inlineStr">
         <is>
-          <t>2022-03-05T09:29:17Z</t>
+          <t>2022-03-12T15:05:42Z</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="12" t="inlineStr">
         <is>
-          <t>114 Attributes part 1</t>
+          <t>116 Cow part 2</t>
         </is>
       </c>
       <c r="B119" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=uvJGGBhBfgI</t>
+          <t>https://www.youtube.com/watch?v=yvrRv1dUmLI</t>
         </is>
       </c>
       <c r="C119" s="14" t="inlineStr">
         <is>
-          <t>00:09:36</t>
+          <t>00:08:29</t>
         </is>
       </c>
       <c r="D119" s="10" t="inlineStr">
         <is>
-          <t>2022-03-12T08:12:08Z</t>
+          <t>2022-03-12T15:21:51Z</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="12" t="inlineStr">
         <is>
-          <t>115 Attributes part 2</t>
+          <t>117 Deref trait</t>
         </is>
       </c>
       <c r="B120" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=s1A84oJCp20</t>
+          <t>https://www.youtube.com/watch?v=tFC8ZWvMDOE</t>
         </is>
       </c>
       <c r="C120" s="14" t="inlineStr">
         <is>
-          <t>00:11:07</t>
+          <t>00:10:12</t>
         </is>
       </c>
       <c r="D120" s="10" t="inlineStr">
         <is>
-          <t>2022-03-12T15:05:42Z</t>
+          <t>2022-03-12T15:27:18Z</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="12" t="inlineStr">
         <is>
-          <t>116 Cow part 2</t>
+          <t>118 Deref again</t>
         </is>
       </c>
       <c r="B121" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=yvrRv1dUmLI</t>
+          <t>https://www.youtube.com/watch?v=A5hQZKBZhE0</t>
         </is>
       </c>
       <c r="C121" s="14" t="inlineStr">
         <is>
-          <t>00:08:29</t>
+          <t>00:06:56</t>
         </is>
       </c>
       <c r="D121" s="10" t="inlineStr">
         <is>
-          <t>2022-03-12T15:21:51Z</t>
+          <t>2022-03-12T15:29:29Z</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="12" t="inlineStr">
         <is>
-          <t>117 Deref trait</t>
+          <t>119 Cow in practice</t>
         </is>
       </c>
       <c r="B122" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=tFC8ZWvMDOE</t>
+          <t>https://www.youtube.com/watch?v=1UrSBfjZaU0</t>
         </is>
       </c>
       <c r="C122" s="14" t="inlineStr">
         <is>
-          <t>00:10:12</t>
+          <t>00:06:26</t>
         </is>
       </c>
       <c r="D122" s="10" t="inlineStr">
         <is>
-          <t>2022-03-12T15:27:18Z</t>
+          <t>2022-03-12T15:30:56Z</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="12" t="inlineStr">
         <is>
-          <t>118 Deref again</t>
+          <t>120 to_mut with Cow</t>
         </is>
       </c>
       <c r="B123" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=A5hQZKBZhE0</t>
+          <t>https://www.youtube.com/watch?v=0m45e3UsRGs</t>
         </is>
       </c>
       <c r="C123" s="14" t="inlineStr">
         <is>
-          <t>00:06:56</t>
+          <t>00:06:51</t>
         </is>
       </c>
       <c r="D123" s="10" t="inlineStr">
         <is>
-          <t>2022-03-12T15:29:29Z</t>
+          <t>2022-03-12T15:33:03Z</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="12" t="inlineStr">
         <is>
-          <t>119 Cow in practice</t>
+          <t>121 Add trait</t>
         </is>
       </c>
       <c r="B124" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=1UrSBfjZaU0</t>
+          <t>https://www.youtube.com/watch?v=WpRtLfsr-vg</t>
         </is>
       </c>
       <c r="C124" s="14" t="inlineStr">
         <is>
-          <t>00:06:26</t>
+          <t>00:09:35</t>
         </is>
       </c>
       <c r="D124" s="10" t="inlineStr">
         <is>
-          <t>2022-03-12T15:30:56Z</t>
+          <t>2022-03-19T07:15:50Z</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="12" t="inlineStr">
         <is>
-          <t>120 to_mut with Cow</t>
+          <t>122 Default trait</t>
         </is>
       </c>
       <c r="B125" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=0m45e3UsRGs</t>
+          <t>https://www.youtube.com/watch?v=9iwFUXzJ-xY</t>
         </is>
       </c>
       <c r="C125" s="14" t="inlineStr">
         <is>
-          <t>00:06:51</t>
+          <t>00:10:25</t>
         </is>
       </c>
       <c r="D125" s="10" t="inlineStr">
         <is>
-          <t>2022-03-12T15:33:03Z</t>
+          <t>2022-03-19T07:20:17Z</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="12" t="inlineStr">
         <is>
-          <t>121 Add trait</t>
+          <t>123 Builder pattern</t>
         </is>
       </c>
       <c r="B126" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=WpRtLfsr-vg</t>
+          <t>https://www.youtube.com/watch?v=8As8DMybFpM</t>
         </is>
       </c>
       <c r="C126" s="14" t="inlineStr">
         <is>
-          <t>00:09:35</t>
+          <t>00:08:53</t>
         </is>
       </c>
       <c r="D126" s="10" t="inlineStr">
         <is>
-          <t>2022-03-19T07:15:50Z</t>
+          <t>2022-03-19T07:21:57Z</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="12" t="inlineStr">
         <is>
-          <t>122 Default trait</t>
+          <t>124 Builder pattern 2</t>
         </is>
       </c>
       <c r="B127" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=9iwFUXzJ-xY</t>
+          <t>https://www.youtube.com/watch?v=1hUBNuFMX5Y</t>
         </is>
       </c>
       <c r="C127" s="14" t="inlineStr">
         <is>
-          <t>00:10:25</t>
+          <t>00:13:20</t>
         </is>
       </c>
       <c r="D127" s="10" t="inlineStr">
         <is>
-          <t>2022-03-19T07:20:17Z</t>
+          <t>2022-03-19T07:38:29Z</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="12" t="inlineStr">
         <is>
-          <t>123 Builder pattern</t>
+          <t>125 Test-driven development</t>
         </is>
       </c>
       <c r="B128" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=8As8DMybFpM</t>
+          <t>https://www.youtube.com/watch?v=p8tfNr_uK2g</t>
         </is>
       </c>
       <c r="C128" s="14" t="inlineStr">
         <is>
-          <t>00:08:53</t>
+          <t>00:08:19</t>
         </is>
       </c>
       <c r="D128" s="10" t="inlineStr">
         <is>
-          <t>2022-03-19T07:21:57Z</t>
+          <t>2022-03-19T07:40:30Z</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="12" t="inlineStr">
         <is>
-          <t>124 Builder pattern 2</t>
+          <t>126 Test-driven development 2</t>
         </is>
       </c>
       <c r="B129" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=1hUBNuFMX5Y</t>
+          <t>https://www.youtube.com/watch?v=v2gDoTMtGCw</t>
         </is>
       </c>
       <c r="C129" s="14" t="inlineStr">
         <is>
-          <t>00:13:20</t>
+          <t>00:11:54</t>
         </is>
       </c>
       <c r="D129" s="10" t="inlineStr">
         <is>
-          <t>2022-03-19T07:38:29Z</t>
+          <t>2022-03-19T07:47:46Z</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="12" t="inlineStr">
         <is>
-          <t>125 Test-driven development</t>
+          <t>127 Test-driven development 3</t>
         </is>
       </c>
       <c r="B130" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=p8tfNr_uK2g</t>
+          <t>https://www.youtube.com/watch?v=TQZTZEbx9iM</t>
         </is>
       </c>
       <c r="C130" s="14" t="inlineStr">
         <is>
-          <t>00:08:19</t>
+          <t>00:10:04</t>
         </is>
       </c>
       <c r="D130" s="10" t="inlineStr">
         <is>
-          <t>2022-03-19T07:40:30Z</t>
+          <t>2022-03-19T07:48:50Z</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="12" t="inlineStr">
         <is>
-          <t>126 Test-driven development 2</t>
+          <t>128 Test-driven development 4</t>
         </is>
       </c>
       <c r="B131" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=v2gDoTMtGCw</t>
+          <t>https://www.youtube.com/watch?v=GU_N95-y97w</t>
         </is>
       </c>
       <c r="C131" s="14" t="inlineStr">
         <is>
-          <t>00:11:54</t>
+          <t>00:09:00</t>
         </is>
       </c>
       <c r="D131" s="10" t="inlineStr">
         <is>
-          <t>2022-03-19T07:47:46Z</t>
+          <t>2022-03-19T08:02:07Z</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="12" t="inlineStr">
         <is>
-          <t>127 Test-driven development 3</t>
+          <t>129 Clippy again</t>
         </is>
       </c>
       <c r="B132" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=TQZTZEbx9iM</t>
+          <t>https://www.youtube.com/watch?v=i0kinp6iegg</t>
         </is>
       </c>
       <c r="C132" s="14" t="inlineStr">
         <is>
-          <t>00:10:04</t>
+          <t>00:09:19</t>
         </is>
       </c>
       <c r="D132" s="10" t="inlineStr">
         <is>
-          <t>2022-03-19T07:48:50Z</t>
+          <t>2022-03-27T09:09:25Z</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="12" t="inlineStr">
         <is>
-          <t>128 Test-driven development 4</t>
+          <t>130 Refactoring</t>
         </is>
       </c>
       <c r="B133" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=GU_N95-y97w</t>
+          <t>https://www.youtube.com/watch?v=-jv7fKxVooI</t>
         </is>
       </c>
       <c r="C133" s="14" t="inlineStr">
         <is>
-          <t>00:09:00</t>
+          <t>00:07:25</t>
         </is>
       </c>
       <c r="D133" s="10" t="inlineStr">
         <is>
-          <t>2022-03-19T08:02:07Z</t>
+          <t>2022-03-28T04:47:05Z</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="12" t="inlineStr">
         <is>
-          <t>129 Clippy again</t>
+          <t>131 Refactoring 2</t>
         </is>
       </c>
       <c r="B134" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=i0kinp6iegg</t>
+          <t>https://www.youtube.com/watch?v=jcyUnpNNdbU</t>
         </is>
       </c>
       <c r="C134" s="14" t="inlineStr">
         <is>
-          <t>00:09:19</t>
+          <t>00:09:41</t>
         </is>
       </c>
       <c r="D134" s="10" t="inlineStr">
         <is>
-          <t>2022-03-27T09:09:25Z</t>
+          <t>2022-03-29T12:54:34Z</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="12" t="inlineStr">
         <is>
-          <t>130 Refactoring</t>
+          <t>132 The Any trait</t>
         </is>
       </c>
       <c r="B135" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=-jv7fKxVooI</t>
+          <t>https://www.youtube.com/watch?v=xaYtNn_iH-c</t>
         </is>
       </c>
       <c r="C135" s="14" t="inlineStr">
         <is>
-          <t>00:07:25</t>
+          <t>00:08:57</t>
         </is>
       </c>
       <c r="D135" s="10" t="inlineStr">
         <is>
-          <t>2022-03-28T04:47:05Z</t>
+          <t>2022-03-30T01:46:39Z</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="12" t="inlineStr">
         <is>
-          <t>131 Refactoring 2</t>
+          <t>133 The Any trait 2</t>
         </is>
       </c>
       <c r="B136" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=jcyUnpNNdbU</t>
+          <t>https://www.youtube.com/watch?v=NwvyYG_qDlg</t>
         </is>
       </c>
       <c r="C136" s="14" t="inlineStr">
         <is>
-          <t>00:09:41</t>
+          <t>00:09:02</t>
         </is>
       </c>
       <c r="D136" s="10" t="inlineStr">
         <is>
-          <t>2022-03-29T12:54:34Z</t>
+          <t>2022-04-05T14:58:15Z</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="12" t="inlineStr">
         <is>
-          <t>132 The Any trait</t>
+          <t>134 Panic hooks</t>
         </is>
       </c>
       <c r="B137" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=xaYtNn_iH-c</t>
+          <t>https://www.youtube.com/watch?v=VWbDRPLAaJs</t>
         </is>
       </c>
       <c r="C137" s="14" t="inlineStr">
         <is>
-          <t>00:08:57</t>
+          <t>00:12:18</t>
         </is>
       </c>
       <c r="D137" s="10" t="inlineStr">
         <is>
-          <t>2022-03-30T01:46:39Z</t>
+          <t>2022-04-01T07:51:39Z</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="12" t="inlineStr">
         <is>
-          <t>133 The Any trait 2</t>
+          <t>135 Time</t>
         </is>
       </c>
       <c r="B138" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=NwvyYG_qDlg</t>
+          <t>https://www.youtube.com/watch?v=b-yfdKIxIZw</t>
         </is>
       </c>
       <c r="C138" s="14" t="inlineStr">
         <is>
-          <t>00:09:02</t>
+          <t>00:09:41</t>
         </is>
       </c>
       <c r="D138" s="10" t="inlineStr">
         <is>
-          <t>2022-04-05T14:58:15Z</t>
+          <t>2022-04-02T08:13:38Z</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="12" t="inlineStr">
         <is>
-          <t>134 Panic hooks</t>
+          <t>136 Channels</t>
         </is>
       </c>
       <c r="B139" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=VWbDRPLAaJs</t>
+          <t>https://www.youtube.com/watch?v=EumJbUTWGF0</t>
         </is>
       </c>
       <c r="C139" s="14" t="inlineStr">
         <is>
-          <t>00:12:18</t>
+          <t>00:09:35</t>
         </is>
       </c>
       <c r="D139" s="10" t="inlineStr">
         <is>
-          <t>2022-04-01T07:51:39Z</t>
+          <t>2022-04-05T14:58:48Z</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="12" t="inlineStr">
         <is>
-          <t>135 Time</t>
+          <t>137 Channels 2</t>
         </is>
       </c>
       <c r="B140" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=b-yfdKIxIZw</t>
+          <t>https://www.youtube.com/watch?v=rmhb5whmKjE</t>
         </is>
       </c>
       <c r="C140" s="14" t="inlineStr">
         <is>
-          <t>00:09:41</t>
+          <t>00:08:28</t>
         </is>
       </c>
       <c r="D140" s="10" t="inlineStr">
         <is>
-          <t>2022-04-02T08:13:38Z</t>
+          <t>2022-04-05T14:59:07Z</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="12" t="inlineStr">
         <is>
-          <t>136 Channels</t>
+          <t>138 Channels and the Any trait</t>
         </is>
       </c>
       <c r="B141" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=EumJbUTWGF0</t>
+          <t>https://www.youtube.com/watch?v=0HUDSGVZcqE</t>
         </is>
       </c>
       <c r="C141" s="14" t="inlineStr">
         <is>
-          <t>00:09:35</t>
+          <t>00:08:38</t>
         </is>
       </c>
       <c r="D141" s="10" t="inlineStr">
         <is>
-          <t>2022-04-05T14:58:48Z</t>
+          <t>2022-04-02T09:22:49Z</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="12" t="inlineStr">
         <is>
-          <t>137 Channels 2</t>
+          <t>139 Errors</t>
         </is>
       </c>
       <c r="B142" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=rmhb5whmKjE</t>
+          <t>https://www.youtube.com/watch?v=hrPO-J_texs</t>
         </is>
       </c>
       <c r="C142" s="14" t="inlineStr">
         <is>
-          <t>00:08:28</t>
+          <t>00:09:50</t>
         </is>
       </c>
       <c r="D142" s="10" t="inlineStr">
         <is>
-          <t>2022-04-05T14:59:07Z</t>
+          <t>2022-04-02T09:25:10Z</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="12" t="inlineStr">
         <is>
-          <t>138 Channels and the Any trait</t>
+          <t>140 Errors 2</t>
         </is>
       </c>
       <c r="B143" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=0HUDSGVZcqE</t>
+          <t>https://www.youtube.com/watch?v=GVm-OinlnAA</t>
         </is>
       </c>
       <c r="C143" s="14" t="inlineStr">
         <is>
-          <t>00:08:38</t>
+          <t>00:08:45</t>
         </is>
       </c>
       <c r="D143" s="10" t="inlineStr">
         <is>
-          <t>2022-04-02T09:22:49Z</t>
+          <t>2022-04-05T14:59:43Z</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="12" t="inlineStr">
         <is>
-          <t>139 Errors</t>
+          <t>141 Anyhow crate</t>
         </is>
       </c>
       <c r="B144" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=hrPO-J_texs</t>
+          <t>https://www.youtube.com/watch?v=Ar9NWLxLwEQ</t>
         </is>
       </c>
       <c r="C144" s="14" t="inlineStr">
         <is>
-          <t>00:09:50</t>
+          <t>00:12:13</t>
         </is>
       </c>
       <c r="D144" s="10" t="inlineStr">
         <is>
-          <t>2022-04-02T09:25:10Z</t>
+          <t>2022-04-02T09:27:50Z</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="12" t="inlineStr">
         <is>
-          <t>140 Errors 2</t>
+          <t>142 Thiserror crate</t>
         </is>
       </c>
       <c r="B145" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=GVm-OinlnAA</t>
+          <t>https://www.youtube.com/watch?v=QrJKqJZ4QJE</t>
         </is>
       </c>
       <c r="C145" s="14" t="inlineStr">
         <is>
-          <t>00:08:45</t>
+          <t>00:09:15</t>
         </is>
       </c>
       <c r="D145" s="10" t="inlineStr">
         <is>
-          <t>2022-04-05T14:59:43Z</t>
+          <t>2022-04-09T07:46:51Z</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="12" t="inlineStr">
         <is>
-          <t>141 Anyhow crate</t>
+          <t>143 Thiserror crate 2</t>
         </is>
       </c>
       <c r="B146" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=Ar9NWLxLwEQ</t>
+          <t>https://www.youtube.com/watch?v=6s_yknGVUb4</t>
         </is>
       </c>
       <c r="C146" s="14" t="inlineStr">
         <is>
-          <t>00:12:13</t>
+          <t>00:09:51</t>
         </is>
       </c>
       <c r="D146" s="10" t="inlineStr">
         <is>
-          <t>2022-04-02T09:27:50Z</t>
+          <t>2022-04-09T07:49:23Z</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="12" t="inlineStr">
         <is>
-          <t>142 Thiserror crate</t>
+          <t>144 Thiserror and Anyhow</t>
         </is>
       </c>
       <c r="B147" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=QrJKqJZ4QJE</t>
+          <t>https://www.youtube.com/watch?v=q5bFEFPDrMs</t>
         </is>
       </c>
       <c r="C147" s="14" t="inlineStr">
         <is>
-          <t>00:09:15</t>
+          <t>00:11:44</t>
         </is>
       </c>
       <c r="D147" s="10" t="inlineStr">
         <is>
-          <t>2022-04-09T07:46:51Z</t>
+          <t>2022-04-09T08:02:11Z</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="12" t="inlineStr">
         <is>
-          <t>143 Thiserror crate 2</t>
+          <t>145 Serde</t>
         </is>
       </c>
       <c r="B148" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=6s_yknGVUb4</t>
+          <t>https://www.youtube.com/watch?v=TvZtGcM9wGU</t>
         </is>
       </c>
       <c r="C148" s="14" t="inlineStr">
         <is>
-          <t>00:09:51</t>
+          <t>00:11:01</t>
         </is>
       </c>
       <c r="D148" s="10" t="inlineStr">
         <is>
-          <t>2022-04-09T07:49:23Z</t>
+          <t>2022-04-09T08:03:41Z</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="12" t="inlineStr">
         <is>
-          <t>144 Thiserror and Anyhow</t>
+          <t>146 Random</t>
         </is>
       </c>
       <c r="B149" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=q5bFEFPDrMs</t>
+          <t>https://www.youtube.com/watch?v=jBd02cX2hnY</t>
         </is>
       </c>
       <c r="C149" s="14" t="inlineStr">
         <is>
-          <t>00:11:44</t>
+          <t>00:09:35</t>
         </is>
       </c>
       <c r="D149" s="10" t="inlineStr">
         <is>
-          <t>2022-04-09T08:02:11Z</t>
+          <t>2022-04-09T08:05:06Z</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="12" t="inlineStr">
         <is>
-          <t>145 Serde</t>
+          <t>147 Std library tour 1</t>
         </is>
       </c>
       <c r="B150" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=TvZtGcM9wGU</t>
+          <t>https://www.youtube.com/watch?v=BIB15R0_yHI</t>
         </is>
       </c>
       <c r="C150" s="14" t="inlineStr">
         <is>
-          <t>00:11:01</t>
+          <t>00:10:55</t>
         </is>
       </c>
       <c r="D150" s="10" t="inlineStr">
         <is>
-          <t>2022-04-09T08:03:41Z</t>
+          <t>2022-04-14T07:19:14Z</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="12" t="inlineStr">
         <is>
-          <t>146 Random</t>
+          <t>148 Std library tour 2</t>
         </is>
       </c>
       <c r="B151" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=jBd02cX2hnY</t>
+          <t>https://www.youtube.com/watch?v=INEG9FrOroY</t>
         </is>
       </c>
       <c r="C151" s="14" t="inlineStr">
         <is>
-          <t>00:09:35</t>
+          <t>00:10:13</t>
         </is>
       </c>
       <c r="D151" s="10" t="inlineStr">
         <is>
-          <t>2022-04-09T08:05:06Z</t>
+          <t>2022-04-14T07:22:27Z</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="12" t="inlineStr">
         <is>
-          <t>147 Std library tour 1</t>
+          <t>149 Std library tour 3</t>
         </is>
       </c>
       <c r="B152" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=BIB15R0_yHI</t>
+          <t>https://www.youtube.com/watch?v=GyNRcFRjofo</t>
         </is>
       </c>
       <c r="C152" s="14" t="inlineStr">
         <is>
-          <t>00:10:55</t>
+          <t>00:06:57</t>
         </is>
       </c>
       <c r="D152" s="10" t="inlineStr">
         <is>
-          <t>2022-04-14T07:19:14Z</t>
+          <t>2022-04-16T08:19:55Z</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="12" t="inlineStr">
         <is>
-          <t>148 Std library tour 2</t>
+          <t>150 Leaking Boxes</t>
         </is>
       </c>
       <c r="B153" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=INEG9FrOroY</t>
+          <t>https://www.youtube.com/watch?v=4-FOOCRbjaY</t>
         </is>
       </c>
       <c r="C153" s="14" t="inlineStr">
         <is>
-          <t>00:10:13</t>
+          <t>00:08:47</t>
         </is>
       </c>
       <c r="D153" s="10" t="inlineStr">
         <is>
-          <t>2022-04-14T07:22:27Z</t>
+          <t>2022-04-17T03:31:32Z</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="12" t="inlineStr">
         <is>
-          <t>149 Std library tour 3</t>
+          <t>151 Std library tour 4</t>
         </is>
       </c>
       <c r="B154" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=GyNRcFRjofo</t>
+          <t>https://www.youtube.com/watch?v=asNqW0kbb4s</t>
         </is>
       </c>
       <c r="C154" s="14" t="inlineStr">
         <is>
-          <t>00:06:57</t>
+          <t>00:09:29</t>
         </is>
       </c>
       <c r="D154" s="10" t="inlineStr">
         <is>
-          <t>2022-04-16T08:19:55Z</t>
+          <t>2022-04-17T07:45:47Z</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="12" t="inlineStr">
         <is>
-          <t>150 Leaking Boxes</t>
+          <t>152 Std library tour 5</t>
         </is>
       </c>
       <c r="B155" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=4-FOOCRbjaY</t>
+          <t>https://www.youtube.com/watch?v=A0eiasZsH1E</t>
         </is>
       </c>
       <c r="C155" s="14" t="inlineStr">
         <is>
-          <t>00:08:47</t>
+          <t>00:09:32</t>
         </is>
       </c>
       <c r="D155" s="10" t="inlineStr">
         <is>
-          <t>2022-04-17T03:31:32Z</t>
+          <t>2022-04-17T13:11:06Z</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="12" t="inlineStr">
         <is>
-          <t>151 Std library tour 4</t>
+          <t>153 Std library tour 6</t>
         </is>
       </c>
       <c r="B156" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=asNqW0kbb4s</t>
+          <t>https://www.youtube.com/watch?v=sKjPyum5l5Y</t>
         </is>
       </c>
       <c r="C156" s="14" t="inlineStr">
         <is>
-          <t>00:09:29</t>
+          <t>00:09:23</t>
         </is>
       </c>
       <c r="D156" s="10" t="inlineStr">
         <is>
-          <t>2022-04-17T07:45:47Z</t>
+          <t>2022-04-17T13:12:36Z</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="12" t="inlineStr">
         <is>
-          <t>152 Std library tour 5</t>
+          <t>154 Std library tour 7</t>
         </is>
       </c>
       <c r="B157" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=A0eiasZsH1E</t>
+          <t>https://www.youtube.com/watch?v=tMxstfTqyss</t>
         </is>
       </c>
       <c r="C157" s="14" t="inlineStr">
         <is>
-          <t>00:09:32</t>
+          <t>00:09:43</t>
         </is>
       </c>
       <c r="D157" s="10" t="inlineStr">
         <is>
-          <t>2022-04-17T13:11:06Z</t>
+          <t>2022-04-17T13:30:44Z</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="12" t="inlineStr">
         <is>
-          <t>153 Std library tour 6</t>
+          <t>155 Std library tour 8</t>
         </is>
       </c>
       <c r="B158" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=sKjPyum5l5Y</t>
+          <t>https://www.youtube.com/watch?v=yX4nD7iLv84</t>
         </is>
       </c>
       <c r="C158" s="14" t="inlineStr">
         <is>
-          <t>00:09:23</t>
+          <t>00:11:32</t>
         </is>
       </c>
       <c r="D158" s="10" t="inlineStr">
         <is>
-          <t>2022-04-17T13:12:36Z</t>
+          <t>2022-04-17T13:33:56Z</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="12" t="inlineStr">
         <is>
-          <t>154 Std library tour 7</t>
+          <t>156 Std library tour 9</t>
         </is>
       </c>
       <c r="B159" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=tMxstfTqyss</t>
+          <t>https://www.youtube.com/watch?v=thHgqH6fO-E</t>
         </is>
       </c>
       <c r="C159" s="14" t="inlineStr">
         <is>
-          <t>00:09:43</t>
+          <t>00:09:57</t>
         </is>
       </c>
       <c r="D159" s="10" t="inlineStr">
         <is>
-          <t>2022-04-17T13:30:44Z</t>
+          <t>2022-04-23T08:11:53Z</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="12" t="inlineStr">
         <is>
-          <t>155 Std library tour 8</t>
+          <t>157 Macros 1</t>
         </is>
       </c>
       <c r="B160" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=yX4nD7iLv84</t>
+          <t>https://www.youtube.com/watch?v=TvNFCN6gdJU</t>
         </is>
       </c>
       <c r="C160" s="14" t="inlineStr">
         <is>
-          <t>00:11:32</t>
+          <t>00:09:08</t>
         </is>
       </c>
       <c r="D160" s="10" t="inlineStr">
         <is>
-          <t>2022-04-17T13:33:56Z</t>
+          <t>2022-04-23T15:40:20Z</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="12" t="inlineStr">
         <is>
-          <t>156 Std library tour 9</t>
+          <t>158 Macros 2</t>
         </is>
       </c>
       <c r="B161" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=thHgqH6fO-E</t>
+          <t>https://www.youtube.com/watch?v=vq4w6wM2A-0</t>
         </is>
       </c>
       <c r="C161" s="14" t="inlineStr">
         <is>
-          <t>00:09:57</t>
+          <t>00:10:54</t>
         </is>
       </c>
       <c r="D161" s="10" t="inlineStr">
         <is>
-          <t>2022-04-23T08:11:53Z</t>
+          <t>2022-04-24T05:16:54Z</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="12" t="inlineStr">
         <is>
-          <t>157 Macros 1</t>
+          <t>159 Macros 3</t>
         </is>
       </c>
       <c r="B162" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=TvNFCN6gdJU</t>
+          <t>https://www.youtube.com/watch?v=9RpfuEeFa-M</t>
         </is>
       </c>
       <c r="C162" s="14" t="inlineStr">
         <is>
-          <t>00:09:08</t>
+          <t>00:11:25</t>
         </is>
       </c>
       <c r="D162" s="10" t="inlineStr">
         <is>
-          <t>2022-04-23T15:40:20Z</t>
+          <t>2022-04-24T05:17:59Z</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="12" t="inlineStr">
         <is>
-          <t>158 Macros 2</t>
+          <t>160 Macros 4</t>
         </is>
       </c>
       <c r="B163" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=vq4w6wM2A-0</t>
+          <t>https://www.youtube.com/watch?v=iiSBee6GqWI</t>
         </is>
       </c>
       <c r="C163" s="14" t="inlineStr">
         <is>
-          <t>00:10:54</t>
+          <t>00:09:51</t>
         </is>
       </c>
       <c r="D163" s="10" t="inlineStr">
         <is>
-          <t>2022-04-24T05:16:54Z</t>
+          <t>2022-04-24T06:21:06Z</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="12" t="inlineStr">
         <is>
-          <t>159 Macros 3</t>
+          <t>161 Const generics</t>
         </is>
       </c>
       <c r="B164" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=9RpfuEeFa-M</t>
+          <t>https://www.youtube.com/watch?v=4474b493qnE</t>
         </is>
       </c>
       <c r="C164" s="14" t="inlineStr">
         <is>
-          <t>00:11:25</t>
+          <t>00:09:02</t>
         </is>
       </c>
       <c r="D164" s="10" t="inlineStr">
         <is>
-          <t>2022-04-24T05:17:59Z</t>
+          <t>2022-04-24T06:24:40Z</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="12" t="inlineStr">
         <is>
-          <t>160 Macros 4</t>
+          <t>162 Const functions</t>
         </is>
       </c>
       <c r="B165" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=iiSBee6GqWI</t>
+          <t>https://www.youtube.com/watch?v=7XDAM8yVYBk</t>
         </is>
       </c>
       <c r="C165" s="14" t="inlineStr">
         <is>
-          <t>00:09:51</t>
+          <t>00:08:21</t>
         </is>
       </c>
       <c r="D165" s="10" t="inlineStr">
         <is>
-          <t>2022-04-24T06:21:06Z</t>
+          <t>2022-04-24T06:27:04Z</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="12" t="inlineStr">
         <is>
-          <t>161 Const generics</t>
+          <t>163 lazy_static</t>
         </is>
       </c>
       <c r="B166" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=4474b493qnE</t>
+          <t>https://www.youtube.com/watch?v=So6lEjUjsoU</t>
         </is>
       </c>
       <c r="C166" s="14" t="inlineStr">
         <is>
-          <t>00:09:02</t>
+          <t>00:07:05</t>
         </is>
       </c>
       <c r="D166" s="10" t="inlineStr">
         <is>
-          <t>2022-04-24T06:24:40Z</t>
+          <t>2022-04-30T08:05:51Z</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="12" t="inlineStr">
         <is>
-          <t>162 Const functions</t>
+          <t>164 OneCell</t>
         </is>
       </c>
       <c r="B167" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=7XDAM8yVYBk</t>
+          <t>https://www.youtube.com/watch?v=o5QZwVZYygM</t>
         </is>
       </c>
       <c r="C167" s="14" t="inlineStr">
         <is>
-          <t>00:08:21</t>
+          <t>00:09:16</t>
         </is>
       </c>
       <c r="D167" s="10" t="inlineStr">
         <is>
-          <t>2022-04-24T06:27:04Z</t>
+          <t>2022-04-30T14:26:01Z</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="12" t="inlineStr">
         <is>
-          <t>163 lazy_static</t>
+          <t>165 Installing Rust</t>
         </is>
       </c>
       <c r="B168" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=So6lEjUjsoU</t>
+          <t>https://www.youtube.com/watch?v=gOJyMiNXXB0</t>
         </is>
       </c>
       <c r="C168" s="14" t="inlineStr">
         <is>
-          <t>00:07:05</t>
+          <t>00:09:51</t>
         </is>
       </c>
       <c r="D168" s="10" t="inlineStr">
         <is>
-          <t>2022-04-30T08:05:51Z</t>
+          <t>2022-05-01T15:52:51Z</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="12" t="inlineStr">
         <is>
-          <t>164 OneCell</t>
+          <t>166 Rust and VS Code</t>
         </is>
       </c>
       <c r="B169" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=o5QZwVZYygM</t>
+          <t>https://www.youtube.com/watch?v=0nXi7er7j30</t>
         </is>
       </c>
       <c r="C169" s="14" t="inlineStr">
         <is>
-          <t>00:09:16</t>
+          <t>00:10:50</t>
         </is>
       </c>
       <c r="D169" s="10" t="inlineStr">
         <is>
-          <t>2022-04-30T14:26:01Z</t>
+          <t>2022-05-02T13:39:20Z</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="12" t="inlineStr">
         <is>
-          <t>165 Installing Rust</t>
+          <t>167 Reqwest 1</t>
         </is>
       </c>
       <c r="B170" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=gOJyMiNXXB0</t>
+          <t>https://www.youtube.com/watch?v=hjOg2u932jg</t>
         </is>
       </c>
       <c r="C170" s="14" t="inlineStr">
         <is>
-          <t>00:09:51</t>
+          <t>00:09:24</t>
         </is>
       </c>
       <c r="D170" s="10" t="inlineStr">
         <is>
-          <t>2022-05-01T15:52:51Z</t>
+          <t>2022-05-03T14:15:52Z</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="12" t="inlineStr">
         <is>
-          <t>166 Rust and VS Code</t>
+          <t>168 Reqwest 2</t>
         </is>
       </c>
       <c r="B171" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=0nXi7er7j30</t>
+          <t>https://www.youtube.com/watch?v=GZPtFAJD0ws</t>
         </is>
       </c>
       <c r="C171" s="14" t="inlineStr">
         <is>
-          <t>00:10:50</t>
+          <t>00:09:31</t>
         </is>
       </c>
       <c r="D171" s="10" t="inlineStr">
         <is>
-          <t>2022-05-02T13:39:20Z</t>
+          <t>2022-05-03T14:17:19Z</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="12" t="inlineStr">
         <is>
-          <t>167 Reqwest 1</t>
+          <t>169 async</t>
         </is>
       </c>
       <c r="B172" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=hjOg2u932jg</t>
+          <t>https://www.youtube.com/watch?v=xrPdkaVMxpI</t>
         </is>
       </c>
       <c r="C172" s="14" t="inlineStr">
         <is>
-          <t>00:09:24</t>
+          <t>00:10:00</t>
         </is>
       </c>
       <c r="D172" s="10" t="inlineStr">
         <is>
-          <t>2022-05-03T14:15:52Z</t>
+          <t>2022-05-03T14:18:42Z</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="12" t="inlineStr">
         <is>
-          <t>168 Reqwest 2</t>
+          <t>170 fn and async fn</t>
         </is>
       </c>
       <c r="B173" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=GZPtFAJD0ws</t>
+          <t>https://www.youtube.com/watch?v=TOJf9b9jn7I</t>
         </is>
       </c>
       <c r="C173" s="14" t="inlineStr">
         <is>
-          <t>00:09:31</t>
+          <t>00:08:42</t>
         </is>
       </c>
       <c r="D173" s="10" t="inlineStr">
         <is>
-          <t>2022-05-03T14:17:19Z</t>
+          <t>2022-05-21T06:38:52Z</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="12" t="inlineStr">
         <is>
-          <t>169 async</t>
+          <t>171 True async</t>
         </is>
       </c>
       <c r="B174" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=xrPdkaVMxpI</t>
+          <t>https://www.youtube.com/watch?v=tDVCPc-EGZQ</t>
         </is>
       </c>
       <c r="C174" s="14" t="inlineStr">
         <is>
-          <t>00:10:00</t>
+          <t>00:09:42</t>
         </is>
       </c>
       <c r="D174" s="10" t="inlineStr">
         <is>
-          <t>2022-05-03T14:18:42Z</t>
+          <t>2022-05-21T06:40:45Z</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="12" t="inlineStr">
         <is>
-          <t>170 fn and async fn</t>
+          <t>172 tokio select</t>
         </is>
       </c>
       <c r="B175" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=TOJf9b9jn7I</t>
+          <t>https://www.youtube.com/watch?v=rGR1jNsE__4</t>
         </is>
       </c>
       <c r="C175" s="14" t="inlineStr">
         <is>
-          <t>00:08:42</t>
+          <t>00:08:52</t>
         </is>
       </c>
       <c r="D175" s="10" t="inlineStr">
         <is>
-          <t>2022-05-21T06:38:52Z</t>
+          <t>2022-05-21T06:41:56Z</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="12" t="inlineStr">
         <is>
-          <t>171 True async</t>
+          <t>173 User input</t>
         </is>
       </c>
       <c r="B176" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=tDVCPc-EGZQ</t>
+          <t>https://www.youtube.com/watch?v=SsUVRbmHoZE</t>
         </is>
       </c>
       <c r="C176" s="14" t="inlineStr">
         <is>
-          <t>00:09:42</t>
+          <t>00:10:20</t>
         </is>
       </c>
       <c r="D176" s="10" t="inlineStr">
         <is>
-          <t>2022-05-21T06:40:45Z</t>
+          <t>2022-06-19T07:09:38Z</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="12" t="inlineStr">
         <is>
-          <t>172 tokio select</t>
+          <t>174 Program arguments</t>
         </is>
       </c>
       <c r="B177" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=rGR1jNsE__4</t>
+          <t>https://www.youtube.com/watch?v=PLqe4vD2iVg</t>
         </is>
       </c>
       <c r="C177" s="14" t="inlineStr">
         <is>
-          <t>00:08:52</t>
+          <t>00:13:12</t>
         </is>
       </c>
       <c r="D177" s="10" t="inlineStr">
         <is>
-          <t>2022-05-21T06:41:56Z</t>
+          <t>2022-06-19T07:11:45Z</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="12" t="inlineStr">
         <is>
-          <t>173 User input</t>
+          <t>175 Statics in Rust 1.63</t>
         </is>
       </c>
       <c r="B178" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=SsUVRbmHoZE</t>
+          <t>https://www.youtube.com/watch?v=T5OwV2HaH9E</t>
         </is>
       </c>
       <c r="C178" s="14" t="inlineStr">
         <is>
-          <t>00:10:20</t>
+          <t>00:09:31</t>
         </is>
       </c>
       <c r="D178" s="10" t="inlineStr">
         <is>
-          <t>2022-06-19T07:09:38Z</t>
+          <t>2022-06-26T06:40:20Z</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="12" t="inlineStr">
         <is>
-          <t>174 Program arguments</t>
+          <t>176 Environment variables</t>
         </is>
       </c>
       <c r="B179" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=PLqe4vD2iVg</t>
+          <t>https://www.youtube.com/watch?v=-6SILVWuG5g</t>
         </is>
       </c>
       <c r="C179" s="14" t="inlineStr">
         <is>
-          <t>00:13:12</t>
+          <t>00:08:09</t>
         </is>
       </c>
       <c r="D179" s="10" t="inlineStr">
         <is>
-          <t>2022-06-19T07:11:45Z</t>
+          <t>2022-06-26T06:43:30Z</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="12" t="inlineStr">
         <is>
-          <t>175 Statics in Rust 1.63</t>
+          <t>177 Scoped threads</t>
         </is>
       </c>
       <c r="B180" s="13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=T5OwV2HaH9E</t>
+          <t>https://www.youtube.com/watch?v=FfZJd-bpGdc</t>
         </is>
       </c>
       <c r="C180" s="14" t="inlineStr">
         <is>
-          <t>00:09:31</t>
+          <t>00:12:17</t>
         </is>
       </c>
       <c r="D180" s="10" t="inlineStr">
         <is>
-          <t>2022-06-26T06:40:20Z</t>
-        </is>
-      </c>
-    </row>
-    <row r="181">
-      <c r="A181" s="12" t="inlineStr">
-        <is>
-          <t>176 Environment variables</t>
-        </is>
-      </c>
-      <c r="B181" s="13" t="inlineStr">
-        <is>
-          <t>https://www.youtube.com/watch?v=-6SILVWuG5g</t>
-        </is>
-      </c>
-      <c r="C181" s="14" t="inlineStr">
-        <is>
-          <t>00:08:09</t>
-        </is>
-      </c>
-      <c r="D181" s="10" t="inlineStr">
-        <is>
-          <t>2022-06-26T06:43:30Z</t>
-        </is>
-      </c>
-    </row>
-    <row r="182">
-      <c r="A182" s="12" t="inlineStr">
-        <is>
-          <t>177 Scoped threads</t>
-        </is>
-      </c>
-      <c r="B182" s="13" t="inlineStr">
-        <is>
-          <t>https://www.youtube.com/watch?v=FfZJd-bpGdc</t>
-        </is>
-      </c>
-      <c r="C182" s="14" t="inlineStr">
-        <is>
-          <t>00:12:17</t>
-        </is>
-      </c>
-      <c r="D182" s="10" t="inlineStr">
-        <is>
           <t>2022-07-10T07:55:48Z</t>
-        </is>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="12" t="inlineStr">
-        <is>
-          <t>CompComputer can't handle live streaming</t>
-        </is>
-      </c>
-      <c r="B183" s="13" t="inlineStr">
-        <is>
-          <t>https://www.youtube.com/watch?v=uxVw4qIDxRM</t>
-        </is>
-      </c>
-      <c r="C183" s="14" t="inlineStr">
-        <is>
-          <t>00:01:20</t>
-        </is>
-      </c>
-      <c r="D183" s="10" t="inlineStr">
-        <is>
-          <t>2022-05-08T07:10:01Z</t>
-        </is>
-      </c>
-    </row>
-    <row r="184">
-      <c r="A184" s="12" t="inlineStr">
-        <is>
-          <t>이번 주이번 주말에 Easy Rust 더 찍도록 하겠습니다. Working on a new Easy Rust project!</t>
-        </is>
-      </c>
-      <c r="B184" s="13" t="inlineStr">
-        <is>
-          <t>https://www.youtube.com/watch?v=eSFaEWdTdEk</t>
-        </is>
-      </c>
-      <c r="C184" s="14" t="inlineStr">
-        <is>
-          <t>00:01:11</t>
-        </is>
-      </c>
-      <c r="D184" s="10" t="inlineStr">
-        <is>
-          <t>2022-07-06T14:18:54Z</t>
         </is>
       </c>
     </row>
@@ -4722,10 +4638,6 @@
     <hyperlink ref="B178" r:id="rId176"/>
     <hyperlink ref="B179" r:id="rId177"/>
     <hyperlink ref="B180" r:id="rId178"/>
-    <hyperlink ref="B181" r:id="rId179"/>
-    <hyperlink ref="B182" r:id="rId180"/>
-    <hyperlink ref="B183" r:id="rId181"/>
-    <hyperlink ref="B184" r:id="rId182"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>